<commit_message>
update & fix Kinetis pinout
</commit_message>
<xml_diff>
--- a/pin_map.xlsx
+++ b/pin_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="498">
   <si>
     <t>function</t>
   </si>
@@ -702,15 +702,9 @@
     <t>Engine Speed (Crank sensor -)</t>
   </si>
   <si>
-    <t>MAP sensor Gnd</t>
-  </si>
-  <si>
     <t>O2-sensor Gnd</t>
   </si>
   <si>
-    <t>Manifold pressure</t>
-  </si>
-  <si>
     <t>Engine Coolant Temp. (CLT)</t>
   </si>
   <si>
@@ -906,21 +900,9 @@
     <t>- 1 OSC_IN</t>
   </si>
   <si>
-    <t>SPI1_SIN</t>
-  </si>
-  <si>
-    <t>SPI1_SCK</t>
-  </si>
-  <si>
     <t>SPI1_CS</t>
   </si>
   <si>
-    <t>SPI0_CS</t>
-  </si>
-  <si>
-    <t>SPI0_SOUT</t>
-  </si>
-  <si>
     <t>SPI0_SIN</t>
   </si>
   <si>
@@ -948,12 +930,6 @@
     <t>D16</t>
   </si>
   <si>
-    <t>CMP2_0</t>
-  </si>
-  <si>
-    <t>CMP2_1</t>
-  </si>
-  <si>
     <t>CMP2_2</t>
   </si>
   <si>
@@ -1008,12 +984,6 @@
     <t>CMP1_6/ADC1_6</t>
   </si>
   <si>
-    <t>ADC1_3/FXIO_5</t>
-  </si>
-  <si>
-    <t>SPI1_SOUT/FXIO_4</t>
-  </si>
-  <si>
     <t>SPI1</t>
   </si>
   <si>
@@ -1035,51 +1005,12 @@
     <t>ADC2_5</t>
   </si>
   <si>
-    <t>FXIO_1</t>
-  </si>
-  <si>
-    <t>FXIO_0</t>
-  </si>
-  <si>
-    <t>ADC2_6</t>
-  </si>
-  <si>
-    <t>ADC2_7</t>
-  </si>
-  <si>
     <t>Reset_b</t>
   </si>
   <si>
-    <t>FXIO_3</t>
-  </si>
-  <si>
-    <t>FXIO_2</t>
-  </si>
-  <si>
-    <t>FXIO_4</t>
-  </si>
-  <si>
-    <t>FXIO_5</t>
-  </si>
-  <si>
-    <t>FXIO_7</t>
-  </si>
-  <si>
-    <t>FXIO_6</t>
-  </si>
-  <si>
-    <t>- 6 FXIOs (ignition)</t>
-  </si>
-  <si>
     <t>SPI0</t>
   </si>
   <si>
-    <t>FXIO_3/CMP0_1/ADC0_1</t>
-  </si>
-  <si>
-    <t>FXIO_2/CMP0_0/ADC0_0</t>
-  </si>
-  <si>
     <t>FXIO_5/ADC2_13</t>
   </si>
   <si>
@@ -1371,12 +1302,6 @@
     <t>- 2 USART2 (to Kinetis and K-line)</t>
   </si>
   <si>
-    <t>ADC0_4/UART0_RX</t>
-  </si>
-  <si>
-    <t>ADC0_5/UART0_TX</t>
-  </si>
-  <si>
     <t>ADC1_4/UART1_RX</t>
   </si>
   <si>
@@ -1398,9 +1323,6 @@
     <t>- 4 SPI2-Master (To TLEs and Kinetis)</t>
   </si>
   <si>
-    <t>- 2 FXIOs (digital 5V outputs)</t>
-  </si>
-  <si>
     <t>1_07</t>
   </si>
   <si>
@@ -1488,24 +1410,9 @@
     <t>OUT_TLE7</t>
   </si>
   <si>
-    <t>IN_K &lt;--&gt; OUT_STM</t>
-  </si>
-  <si>
-    <t>OUT_K &lt;--&gt; IN_STM</t>
-  </si>
-  <si>
     <t>- 2 GPIO-out (to Kinetis, to TLE7*)</t>
   </si>
   <si>
-    <t>- 4 SPI0-Slave (From STM)</t>
-  </si>
-  <si>
-    <t>- 4 SPI1-Master (To TLEs)</t>
-  </si>
-  <si>
-    <t>* Kinetis-SPI1 is in Master-mode, used only if STM is absent</t>
-  </si>
-  <si>
     <t>GPIO</t>
   </si>
   <si>
@@ -1516,6 +1423,93 @@
   </si>
   <si>
     <t>GNDA</t>
+  </si>
+  <si>
+    <t>Manifold pressure / MAF</t>
+  </si>
+  <si>
+    <t>MAP/MAF sensor Gnd</t>
+  </si>
+  <si>
+    <t>Lambda Sensor 2 In</t>
+  </si>
+  <si>
+    <t>SPI0_SOUT/ADC0_5/UART0_TX</t>
+  </si>
+  <si>
+    <t>HIDRV*</t>
+  </si>
+  <si>
+    <t>* Kinetis-SPI0 is in Master-mode, used only if STM is absent</t>
+  </si>
+  <si>
+    <t>- 4 SPI1-Slave (From STM)</t>
+  </si>
+  <si>
+    <t>- 4 SPI0-Master (To TLEs)</t>
+  </si>
+  <si>
+    <t>*We use SPI1 to connect to STM because of the bootloader</t>
+  </si>
+  <si>
+    <t>GPIO/ADC2_6</t>
+  </si>
+  <si>
+    <t>GPIO/ADC2_7</t>
+  </si>
+  <si>
+    <t>SPI0_CS0/ADC0_4/UART0_RX</t>
+  </si>
+  <si>
+    <t>- 2 GPIOs (digital 5V outputs)</t>
+  </si>
+  <si>
+    <t>HIDRV/SPI0_CS</t>
+  </si>
+  <si>
+    <t>HIDRV/SPI0_SOUT</t>
+  </si>
+  <si>
+    <t>HIDRV/CMP2_0</t>
+  </si>
+  <si>
+    <t>HIDRV/CMP2_1</t>
+  </si>
+  <si>
+    <t>HIDRV/SPI1_SIN</t>
+  </si>
+  <si>
+    <t>HIDRV/SPI1_SCK</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>SPI1_SOUT</t>
+  </si>
+  <si>
+    <t>ADC1_3</t>
+  </si>
+  <si>
+    <t>CMP0_1/ADC0_1</t>
+  </si>
+  <si>
+    <t>CMP0_0/ADC0_0</t>
+  </si>
+  <si>
+    <t>- 6 HI-DRIVE Outputs (ignition)</t>
+  </si>
+  <si>
+    <t>IN_K &lt;-- OUT_STM  (8 trigger signals)</t>
+  </si>
+  <si>
+    <t>OUT_K --&gt; IN_STM  (6 ignition signals)</t>
+  </si>
+  <si>
+    <t>*The green are high-drive pins - ignition outputs (no remap for these!)</t>
+  </si>
+  <si>
+    <t>*The yellow are non-remappable pins (no suitable options)</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1611,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1645,6 +1639,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1737,7 +1737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1829,6 +1829,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2179,7 +2184,7 @@
   <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2195,170 +2200,170 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="41" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>369</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="38" t="s">
-        <v>418</v>
+        <v>395</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>493</v>
+        <v>475</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>372</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="38" t="s">
-        <v>428</v>
+        <v>405</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>370</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>371</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>487</v>
+        <v>461</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>419</v>
+        <v>396</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>492</v>
+        <v>464</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>420</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="38" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>458</v>
+        <v>433</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>421</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="38" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>432</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="38" t="s">
-        <v>459</v>
+        <v>434</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>488</v>
+        <v>462</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>400</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="38" t="s">
-        <v>449</v>
+        <v>426</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>350</v>
+        <v>493</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="39" t="s">
-        <v>441</v>
+        <v>418</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>460</v>
+        <v>481</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>410</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D14" s="38" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>411</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D15" s="39" t="s">
-        <v>430</v>
+        <v>407</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F16" s="38" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F17" s="38" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F18" s="38" t="s">
-        <v>412</v>
+        <v>389</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F19" s="39" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -2367,15 +2372,15 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="35" t="s">
-        <v>473</v>
+        <v>447</v>
       </c>
       <c r="C22" s="45"/>
       <c r="D22" s="35" t="s">
-        <v>474</v>
+        <v>448</v>
       </c>
       <c r="E22" s="45"/>
       <c r="F22" s="35" t="s">
-        <v>475</v>
+        <v>449</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -2396,15 +2401,15 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="35" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="C24" s="45"/>
       <c r="D24" s="35" t="s">
-        <v>392</v>
+        <v>369</v>
       </c>
       <c r="E24" s="45"/>
       <c r="F24" s="35" t="s">
-        <v>422</v>
+        <v>399</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -2428,8 +2433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="N83" sqref="N83"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2480,7 +2485,7 @@
       <c r="S2" s="53"/>
       <c r="T2" s="54"/>
       <c r="U2" s="49" t="s">
-        <v>377</v>
+        <v>354</v>
       </c>
       <c r="V2" s="50"/>
     </row>
@@ -2513,23 +2518,23 @@
         <v>116</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="O3" s="10" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q3" s="22"/>
       <c r="R3" s="22" t="s">
-        <v>374</v>
+        <v>351</v>
       </c>
       <c r="S3" s="23" t="s">
-        <v>375</v>
+        <v>352</v>
       </c>
       <c r="T3" s="23" t="s">
-        <v>376</v>
+        <v>353</v>
       </c>
       <c r="U3" s="23">
         <v>8110</v>
@@ -2540,24 +2545,24 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>464</v>
+        <v>438</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="47" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D4" s="43"/>
       <c r="G4" s="4">
         <v>1</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="21" t="s">
         <v>167</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>296</v>
+        <v>486</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="M4" s="4">
         <v>1</v>
@@ -2566,7 +2571,7 @@
         <v>201</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>405</v>
+        <v>382</v>
       </c>
       <c r="P4" s="12"/>
       <c r="Q4" s="24"/>
@@ -2580,24 +2585,24 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>465</v>
+        <v>439</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="47" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D5" s="43"/>
       <c r="G5" s="4">
         <v>2</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="21" t="s">
         <v>166</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>297</v>
+        <v>487</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="M5" s="4">
         <v>2</v>
@@ -2606,7 +2611,7 @@
         <v>202</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>404</v>
+        <v>381</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="25"/>
@@ -2620,11 +2625,11 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>466</v>
+        <v>440</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="47" t="s">
-        <v>470</v>
+        <v>444</v>
       </c>
       <c r="D6" s="43"/>
       <c r="G6" s="4">
@@ -2633,11 +2638,11 @@
       <c r="H6" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="I6" s="20" t="s">
-        <v>354</v>
+      <c r="I6" s="11" t="s">
+        <v>331</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>347</v>
+        <v>459</v>
       </c>
       <c r="M6" s="4">
         <v>3</v>
@@ -2646,7 +2651,7 @@
         <v>203</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>408</v>
+        <v>385</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="25"/>
@@ -2658,11 +2663,11 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
-        <v>467</v>
+        <v>441</v>
       </c>
       <c r="B7" s="43"/>
       <c r="C7" s="48" t="s">
-        <v>471</v>
+        <v>445</v>
       </c>
       <c r="D7" s="43"/>
       <c r="G7" s="4">
@@ -2671,11 +2676,11 @@
       <c r="H7" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>355</v>
+      <c r="I7" s="11" t="s">
+        <v>332</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>346</v>
+        <v>459</v>
       </c>
       <c r="M7" s="4">
         <v>4</v>
@@ -2684,7 +2689,7 @@
         <v>204</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>406</v>
+        <v>383</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="25"/>
@@ -2698,11 +2703,11 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
-        <v>468</v>
+        <v>442</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="47" t="s">
-        <v>472</v>
+        <v>446</v>
       </c>
       <c r="D8" s="43"/>
       <c r="G8" s="4">
@@ -2712,11 +2717,11 @@
       <c r="H8" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="I8" s="20" t="s">
-        <v>356</v>
+      <c r="I8" s="11" t="s">
+        <v>333</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>348</v>
+        <v>488</v>
       </c>
       <c r="M8" s="4">
         <v>5</v>
@@ -2725,7 +2730,7 @@
         <v>205</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>407</v>
+        <v>384</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="25"/>
@@ -2739,11 +2744,11 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="32" t="s">
-        <v>472</v>
+        <v>446</v>
       </c>
       <c r="D9" s="32"/>
       <c r="G9" s="4">
@@ -2753,11 +2758,11 @@
       <c r="H9" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="I9" s="20" t="s">
-        <v>357</v>
+      <c r="I9" s="11" t="s">
+        <v>334</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>349</v>
+        <v>488</v>
       </c>
       <c r="M9" s="4">
         <v>6</v>
@@ -2766,45 +2771,45 @@
         <v>206</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="Q9" s="25"/>
       <c r="R9" s="25"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="V9" s="5"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>461</v>
+        <v>435</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>182</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="G10" s="32">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H10" s="43" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J10" s="46" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="M10" s="4">
         <v>7</v>
@@ -2813,45 +2818,45 @@
         <v>207</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="P10" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="V10" s="5"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>462</v>
+        <v>436</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>183</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="G11" s="32">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H11" s="43" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="J11" s="46" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="M11" s="4">
         <v>8</v>
@@ -2860,10 +2865,10 @@
         <v>208</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
@@ -2871,46 +2876,46 @@
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>463</v>
+        <v>437</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>184</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="G12" s="32">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H12" s="43" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="I12" s="44" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="J12" s="46" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="M12" s="4">
         <v>9</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="Q12" s="25"/>
       <c r="R12" s="25"/>
@@ -2929,23 +2934,23 @@
         <v>185</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="G13" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="H13" s="43" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="J13" s="44" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="M13" s="4">
         <v>10</v>
@@ -2954,7 +2959,7 @@
         <v>209</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="25"/>
@@ -2974,10 +2979,10 @@
         <v>186</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="0"/>
@@ -2987,20 +2992,20 @@
         <v>141</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="M14" s="4">
         <v>11</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="P14" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="Q14" s="25"/>
       <c r="R14" s="25"/>
@@ -3019,10 +3024,10 @@
         <v>187</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>425</v>
+        <v>402</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="0"/>
@@ -3032,10 +3037,10 @@
         <v>140</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>424</v>
+        <v>401</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="M15" s="4">
         <v>12</v>
@@ -3044,10 +3049,10 @@
         <v>210</v>
       </c>
       <c r="O15" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P15" s="11" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="25"/>
@@ -3064,10 +3069,10 @@
         <v>188</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" si="0"/>
@@ -3077,10 +3082,10 @@
         <v>185</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="M16" s="4">
         <v>13</v>
@@ -3089,13 +3094,13 @@
         <v>211</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>401</v>
+        <v>378</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="25"/>
       <c r="R16" s="25"/>
       <c r="S16" s="5" t="s">
-        <v>387</v>
+        <v>364</v>
       </c>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
@@ -3109,23 +3114,23 @@
         <v>163</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>310</v>
+      <c r="H17" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="I17" s="55" t="s">
+        <v>484</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="M17" s="4">
         <v>14</v>
@@ -3134,7 +3139,7 @@
         <v>212</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="25"/>
@@ -3154,7 +3159,7 @@
         <v>164</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>426</v>
+        <v>403</v>
       </c>
       <c r="D18" s="33" t="s">
         <v>32</v>
@@ -3163,14 +3168,14 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="I18" s="11" t="s">
-        <v>311</v>
+      <c r="I18" s="55" t="s">
+        <v>485</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="M18" s="4">
         <v>15</v>
@@ -3179,7 +3184,7 @@
         <v>213</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="25"/>
@@ -3199,7 +3204,7 @@
         <v>165</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>427</v>
+        <v>404</v>
       </c>
       <c r="D19" s="33" t="s">
         <v>32</v>
@@ -3212,10 +3217,10 @@
         <v>191</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="M19" s="4">
         <v>16</v>
@@ -3224,7 +3229,7 @@
         <v>214</v>
       </c>
       <c r="O19" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="25"/>
@@ -3244,10 +3249,10 @@
         <v>150</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="0"/>
@@ -3257,10 +3262,10 @@
         <v>190</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="M20" s="4">
         <v>17</v>
@@ -3269,7 +3274,7 @@
         <v>215</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>499</v>
+        <v>468</v>
       </c>
       <c r="P20" s="12"/>
       <c r="Q20" s="24"/>
@@ -3288,20 +3293,20 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>480</v>
+        <v>454</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="I21" s="20" t="s">
-        <v>299</v>
+      <c r="I21" s="55" t="s">
+        <v>482</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>351</v>
+        <v>473</v>
       </c>
       <c r="M21" s="4">
         <v>18</v>
@@ -3310,7 +3315,7 @@
         <v>216</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="25"/>
@@ -3333,20 +3338,20 @@
         <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="I22" s="20" t="s">
-        <v>300</v>
+      <c r="I22" s="55" t="s">
+        <v>483</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>351</v>
+        <v>473</v>
       </c>
       <c r="M22" s="4">
         <v>19</v>
@@ -3355,7 +3360,7 @@
         <v>217</v>
       </c>
       <c r="O22" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="25"/>
@@ -3378,7 +3383,7 @@
         <v>18</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="0"/>
@@ -3388,10 +3393,10 @@
         <v>153</v>
       </c>
       <c r="I23" s="20" t="s">
-        <v>455</v>
+        <v>430</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M23" s="4">
         <v>20</v>
@@ -3400,7 +3405,7 @@
         <v>218</v>
       </c>
       <c r="O23" s="12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="P23" s="12"/>
       <c r="Q23" s="24"/>
@@ -3431,17 +3436,17 @@
         <v>152</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>456</v>
+        <v>431</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M24" s="4">
         <v>21</v>
       </c>
       <c r="N24" s="4"/>
       <c r="O24" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="P24" s="12"/>
       <c r="Q24" s="24"/>
@@ -3464,7 +3469,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
@@ -3474,17 +3479,17 @@
         <v>173</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
       <c r="M25" s="4">
         <v>22</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="P25" s="12"/>
       <c r="Q25" s="24"/>
@@ -3506,7 +3511,9 @@
       <c r="C26" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="G26" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3515,10 +3522,10 @@
         <v>172</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
       <c r="M26" s="4">
         <v>23</v>
@@ -3527,7 +3534,7 @@
         <v>219</v>
       </c>
       <c r="O26" s="11" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="25"/>
@@ -3548,7 +3555,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="0"/>
@@ -3558,10 +3565,10 @@
         <v>171</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
       <c r="M27" s="4">
         <v>24</v>
@@ -3587,7 +3594,7 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="0"/>
@@ -3597,10 +3604,10 @@
         <v>151</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>358</v>
+        <v>335</v>
       </c>
       <c r="M28" s="4">
         <v>25</v>
@@ -3609,17 +3616,17 @@
         <v>221</v>
       </c>
       <c r="O28" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="P28" s="11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="25"/>
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
       <c r="U28" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="V28" s="5"/>
     </row>
@@ -3634,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="0"/>
@@ -3644,10 +3651,10 @@
         <v>150</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>359</v>
+        <v>336</v>
       </c>
       <c r="M29" s="4">
         <v>26</v>
@@ -3656,17 +3663,17 @@
         <v>221</v>
       </c>
       <c r="O29" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="P29" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="Q29" s="25"/>
       <c r="R29" s="25"/>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
       <c r="U29" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V29" s="5"/>
     </row>
@@ -3681,20 +3688,20 @@
         <v>6</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M30" s="4">
         <v>27</v>
@@ -3703,17 +3710,17 @@
         <v>222</v>
       </c>
       <c r="O30" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="P30" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="25"/>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
       <c r="U30" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="V30" s="5"/>
     </row>
@@ -3728,29 +3735,29 @@
         <v>7</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M31" s="4">
         <v>28</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="O31" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="25"/>
@@ -3779,10 +3786,10 @@
         <v>165</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M32" s="4">
         <v>29</v>
@@ -3791,10 +3798,10 @@
         <v>223</v>
       </c>
       <c r="O32" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P32" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="25"/>
@@ -3802,7 +3809,7 @@
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
       <c r="V32" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
@@ -3813,10 +3820,10 @@
         <v>155</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>489</v>
+        <v>463</v>
       </c>
       <c r="G33" s="4">
         <f t="shared" si="0"/>
@@ -3826,10 +3833,10 @@
         <v>164</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M33" s="4">
         <v>30</v>
@@ -3863,10 +3870,10 @@
         <v>137</v>
       </c>
       <c r="I34" s="20" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="M34" s="4">
         <v>31</v>
@@ -3875,7 +3882,7 @@
         <v>224</v>
       </c>
       <c r="O34" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P34" s="11"/>
       <c r="Q34" s="25"/>
@@ -3895,10 +3902,10 @@
         <v>135</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>489</v>
+        <v>463</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="0"/>
@@ -3908,10 +3915,10 @@
         <v>136</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="M35" s="4">
         <v>32</v>
@@ -3920,7 +3927,7 @@
         <v>225</v>
       </c>
       <c r="O35" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="P35" s="11"/>
       <c r="Q35" s="25"/>
@@ -3950,11 +3957,11 @@
       <c r="H36" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I36" s="11" t="s">
-        <v>452</v>
+      <c r="I36" s="20" t="s">
+        <v>472</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>360</v>
+        <v>330</v>
       </c>
       <c r="M36" s="4">
         <v>33</v>
@@ -3963,7 +3970,7 @@
         <v>226</v>
       </c>
       <c r="O36" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="P36" s="11"/>
       <c r="Q36" s="25"/>
@@ -3989,11 +3996,11 @@
       <c r="H37" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="I37" s="11" t="s">
-        <v>451</v>
+      <c r="I37" s="20" t="s">
+        <v>480</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>360</v>
+        <v>330</v>
       </c>
       <c r="M37" s="4">
         <v>34</v>
@@ -4002,7 +4009,7 @@
         <v>227</v>
       </c>
       <c r="O37" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="P37" s="11"/>
       <c r="Q37" s="25"/>
@@ -4029,19 +4036,19 @@
         <v>159</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>478</v>
+        <v>452</v>
       </c>
       <c r="M38" s="4">
         <v>35</v>
       </c>
       <c r="N38" s="28" t="s">
-        <v>228</v>
+        <v>470</v>
       </c>
       <c r="O38" s="11" t="s">
-        <v>499</v>
+        <v>468</v>
       </c>
       <c r="P38" s="11"/>
       <c r="Q38" s="25"/>
@@ -4068,19 +4075,19 @@
         <v>158</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>478</v>
+        <v>452</v>
       </c>
       <c r="M39" s="4">
         <v>36</v>
       </c>
       <c r="N39" s="28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O39" s="11" t="s">
-        <v>499</v>
+        <v>468</v>
       </c>
       <c r="P39" s="11"/>
       <c r="Q39" s="25"/>
@@ -4107,22 +4114,22 @@
         <v>125</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>366</v>
+        <v>343</v>
       </c>
       <c r="M40" s="4">
         <v>37</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>230</v>
+        <v>469</v>
       </c>
       <c r="O40" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P40" s="12" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="Q40" s="25"/>
       <c r="R40" s="25"/>
@@ -4141,10 +4148,10 @@
         <v>192</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" si="0"/>
@@ -4154,20 +4161,20 @@
         <v>124</v>
       </c>
       <c r="I41" s="20" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="M41" s="4">
         <v>38</v>
       </c>
       <c r="N41" s="4"/>
       <c r="O41" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P41" s="12" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
       <c r="Q41" s="25"/>
       <c r="R41" s="25"/>
@@ -4186,10 +4193,10 @@
         <v>195</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="0"/>
@@ -4199,19 +4206,19 @@
         <v>189</v>
       </c>
       <c r="I42" s="20" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>361</v>
+        <v>338</v>
       </c>
       <c r="M42" s="4">
         <v>39</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O42" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P42" s="11"/>
       <c r="Q42" s="25"/>
@@ -4231,32 +4238,32 @@
         <v>194</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="G43" s="32">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="H43" s="43" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="I43" s="44" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="J43" s="44" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="M43" s="4">
         <v>40</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="O43" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P43" s="11"/>
       <c r="Q43" s="25"/>
@@ -4276,33 +4283,33 @@
         <v>197</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="G44" s="32">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="H44" s="43" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="I44" s="44" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J44" s="44" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="M44" s="4">
         <v>41</v>
       </c>
       <c r="N44" s="4"/>
       <c r="O44" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P44" s="12" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
       <c r="Q44" s="25"/>
       <c r="R44" s="25"/>
@@ -4321,10 +4328,10 @@
         <v>196</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="0"/>
@@ -4334,22 +4341,22 @@
         <v>147</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M45" s="4">
         <v>42</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="O45" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P45" s="12" t="s">
-        <v>382</v>
+        <v>359</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="25"/>
@@ -4368,10 +4375,10 @@
         <v>145</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>497</v>
+        <v>466</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" si="0"/>
@@ -4381,10 +4388,10 @@
         <v>146</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M46" s="4">
         <v>43</v>
@@ -4407,10 +4414,10 @@
         <v>144</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="G47" s="4">
         <f t="shared" si="0"/>
@@ -4420,19 +4427,19 @@
         <v>170</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="J47" s="11" t="s">
-        <v>365</v>
+        <v>342</v>
       </c>
       <c r="M47" s="4">
         <v>44</v>
       </c>
       <c r="N47" s="19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="O47" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="P47" s="11"/>
       <c r="Q47" s="25"/>
@@ -4450,10 +4457,10 @@
         <v>147</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
       <c r="G48" s="4">
         <f t="shared" si="0"/>
@@ -4463,19 +4470,19 @@
         <v>169</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>330</v>
+        <v>490</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M48" s="4">
         <v>45</v>
       </c>
       <c r="N48" s="19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="O48" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="P48" s="11"/>
       <c r="Q48" s="25"/>
@@ -4496,7 +4503,7 @@
         <v>16</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
       <c r="G49" s="4">
         <f t="shared" si="0"/>
@@ -4506,19 +4513,19 @@
         <v>168</v>
       </c>
       <c r="I49" s="20" t="s">
-        <v>331</v>
+        <v>489</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="M49" s="4">
         <v>46</v>
       </c>
       <c r="N49" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="O49" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P49" s="11"/>
       <c r="Q49" s="25"/>
@@ -4538,11 +4545,9 @@
         <v>149</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>498</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>484</v>
-      </c>
+        <v>467</v>
+      </c>
+      <c r="D50" s="4"/>
       <c r="G50" s="4">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -4551,29 +4556,29 @@
         <v>121</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M50" s="4">
         <v>47</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="O50" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="P50" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="Q50" s="25"/>
       <c r="R50" s="25"/>
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
       <c r="U50" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V50" s="5"/>
     </row>
@@ -4598,19 +4603,19 @@
         <v>120</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M51" s="4">
         <v>48</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O51" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P51" s="11"/>
       <c r="Q51" s="25"/>
@@ -4633,7 +4638,7 @@
         <v>15</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>483</v>
+        <v>457</v>
       </c>
       <c r="G52" s="4">
         <f t="shared" si="0"/>
@@ -4643,10 +4648,10 @@
         <v>119</v>
       </c>
       <c r="I52" s="20" t="s">
-        <v>352</v>
+        <v>491</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="M52" s="4">
         <v>49</v>
@@ -4672,7 +4677,7 @@
         <v>25</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>483</v>
+        <v>457</v>
       </c>
       <c r="G53" s="4">
         <f t="shared" si="0"/>
@@ -4682,19 +4687,19 @@
         <v>118</v>
       </c>
       <c r="I53" s="20" t="s">
-        <v>353</v>
+        <v>492</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="M53" s="4">
         <v>50</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="O53" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P53" s="11"/>
       <c r="Q53" s="25"/>
@@ -4714,10 +4719,10 @@
         <v>177</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
       <c r="G54" s="4">
         <f t="shared" si="0"/>
@@ -4727,10 +4732,10 @@
         <v>157</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>454</v>
+        <v>429</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
       <c r="M54" s="4">
         <v>51</v>
@@ -4739,7 +4744,7 @@
         <v>203</v>
       </c>
       <c r="O54" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="P54" s="11"/>
       <c r="Q54" s="25"/>
@@ -4757,10 +4762,10 @@
         <v>176</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
       <c r="G55" s="4">
         <f t="shared" si="0"/>
@@ -4770,16 +4775,16 @@
         <v>156</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>453</v>
+        <v>428</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
       <c r="M55" s="4">
         <v>52</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
@@ -4798,10 +4803,10 @@
         <v>179</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
       <c r="G56" s="4">
         <f t="shared" si="0"/>
@@ -4811,19 +4816,19 @@
         <v>188</v>
       </c>
       <c r="I56" s="20" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="M56" s="4">
         <v>53</v>
       </c>
       <c r="N56" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O56" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="P56" s="11"/>
       <c r="Q56" s="25"/>
@@ -4841,10 +4846,10 @@
         <v>178</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
       <c r="G57" s="4">
         <f t="shared" si="0"/>
@@ -4854,10 +4859,10 @@
         <v>184</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="J57" s="11" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="M57" s="4">
         <v>54</v>
@@ -4880,10 +4885,10 @@
         <v>181</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
       <c r="G58" s="4">
         <f t="shared" si="0"/>
@@ -4893,19 +4898,19 @@
         <v>131</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>479</v>
+        <v>453</v>
       </c>
       <c r="M58" s="4">
         <v>55</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>216</v>
+        <v>471</v>
       </c>
       <c r="O58" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P58" s="11"/>
       <c r="Q58" s="25"/>
@@ -4925,10 +4930,10 @@
         <v>180</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
       <c r="G59" s="4">
         <f t="shared" si="0"/>
@@ -4938,20 +4943,20 @@
         <v>130</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="J59" s="11" t="s">
-        <v>479</v>
+        <v>453</v>
       </c>
       <c r="M59" s="4">
         <v>56</v>
       </c>
       <c r="N59" s="4"/>
       <c r="O59" s="11" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
       <c r="P59" s="11" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="Q59" s="25"/>
       <c r="R59" s="25"/>
@@ -4979,17 +4984,17 @@
         <v>129</v>
       </c>
       <c r="I60" s="20" t="s">
-        <v>339</v>
+        <v>465</v>
       </c>
       <c r="J60" s="11" t="s">
-        <v>339</v>
+        <v>450</v>
       </c>
       <c r="M60" s="4">
         <v>57</v>
       </c>
       <c r="N60" s="4"/>
       <c r="O60" s="11" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="P60" s="11"/>
       <c r="Q60" s="25"/>
@@ -5018,19 +5023,19 @@
         <v>128</v>
       </c>
       <c r="I61" s="20" t="s">
-        <v>340</v>
+        <v>465</v>
       </c>
       <c r="J61" s="11" t="s">
-        <v>340</v>
+        <v>450</v>
       </c>
       <c r="M61" s="4">
         <v>58</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O61" s="11" t="s">
-        <v>413</v>
+        <v>390</v>
       </c>
       <c r="P61" s="11"/>
       <c r="Q61" s="25"/>
@@ -5057,23 +5062,23 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H62" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="I62" s="11" t="s">
-        <v>341</v>
+      <c r="I62" s="55" t="s">
+        <v>478</v>
       </c>
       <c r="J62" s="11" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="M62" s="4">
         <v>59</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="O62" s="11" t="s">
-        <v>413</v>
+        <v>390</v>
       </c>
       <c r="P62" s="11"/>
       <c r="Q62" s="25"/>
@@ -5100,14 +5105,14 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H63" s="3" t="s">
+      <c r="H63" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="I63" s="11" t="s">
-        <v>342</v>
+      <c r="I63" s="55" t="s">
+        <v>479</v>
       </c>
       <c r="J63" s="11" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="M63" s="4">
         <v>60</v>
@@ -5141,10 +5146,10 @@
         <v>155</v>
       </c>
       <c r="I64" s="11" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="J64" s="11" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
       <c r="M64" s="4">
         <v>61</v>
@@ -5153,7 +5158,7 @@
         <v>203</v>
       </c>
       <c r="O64" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="P64" s="11"/>
       <c r="Q64" s="25"/>
@@ -5182,10 +5187,10 @@
         <v>154</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="J65" s="11" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
       <c r="M65" s="4">
         <v>62</v>
@@ -5221,19 +5226,19 @@
         <v>123</v>
       </c>
       <c r="I66" s="20" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="J66" s="11" t="s">
-        <v>477</v>
+        <v>451</v>
       </c>
       <c r="M66" s="4">
         <v>63</v>
       </c>
       <c r="N66" s="28" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="O66" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="P66" s="11"/>
       <c r="Q66" s="25"/>
@@ -5262,22 +5267,22 @@
         <v>122</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>496</v>
+        <v>465</v>
       </c>
       <c r="J67" s="11" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
       <c r="M67" s="4">
         <v>64</v>
       </c>
       <c r="N67" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="O67" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="P67" s="11" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
       <c r="Q67" s="25"/>
       <c r="R67" s="25"/>
@@ -5303,10 +5308,10 @@
         <v>65</v>
       </c>
       <c r="N68" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="O68" s="11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P68" s="11"/>
       <c r="Q68" s="25"/>
@@ -5330,16 +5335,16 @@
         <v>31</v>
       </c>
       <c r="I69" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="M69" s="4">
         <v>66</v>
       </c>
       <c r="N69" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O69" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="P69" s="11"/>
       <c r="Q69" s="25"/>
@@ -5362,10 +5367,10 @@
         <v>67</v>
       </c>
       <c r="N70" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="O70" s="11" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="P70" s="11"/>
       <c r="Q70" s="25"/>
@@ -5389,16 +5394,16 @@
         <v>28</v>
       </c>
       <c r="G71" t="s">
-        <v>363</v>
+        <v>340</v>
       </c>
       <c r="M71" s="4">
         <v>68</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="O71" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P71" s="11"/>
       <c r="Q71" s="25"/>
@@ -5424,16 +5429,16 @@
         <v>33</v>
       </c>
       <c r="G72" t="s">
-        <v>362</v>
+        <v>339</v>
       </c>
       <c r="M72" s="4">
         <v>69</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O72" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P72" s="13"/>
       <c r="Q72" s="26"/>
@@ -5459,16 +5464,16 @@
         <v>33</v>
       </c>
       <c r="G73" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
       <c r="M73" s="4">
         <v>70</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="O73" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="P73" s="4"/>
       <c r="Q73" s="17"/>
@@ -5494,19 +5499,19 @@
         <v>33</v>
       </c>
       <c r="G74" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="M74" s="4">
         <v>71</v>
       </c>
       <c r="N74" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O74" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="P74" s="4" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="Q74" s="17"/>
       <c r="R74" s="17"/>
@@ -5527,13 +5532,13 @@
       </c>
       <c r="D75" s="29"/>
       <c r="G75" t="s">
-        <v>368</v>
+        <v>345</v>
       </c>
       <c r="M75" s="4">
         <v>72</v>
       </c>
       <c r="N75" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O75" s="4"/>
       <c r="P75" s="4"/>
@@ -5546,7 +5551,7 @@
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="29" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B76" s="30" t="s">
         <v>167</v>
@@ -5556,7 +5561,7 @@
       </c>
       <c r="D76" s="29"/>
       <c r="G76" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
       <c r="M76" s="4">
         <v>73</v>
@@ -5585,19 +5590,19 @@
         <v>33</v>
       </c>
       <c r="G77" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="M77" s="4">
         <v>74</v>
       </c>
       <c r="N77" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="O77" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="P77" s="6" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="Q77" s="17"/>
       <c r="R77" s="17">
@@ -5617,17 +5622,20 @@
       </c>
       <c r="C78" s="29"/>
       <c r="D78" s="29"/>
+      <c r="G78" t="s">
+        <v>477</v>
+      </c>
       <c r="M78" s="4">
         <v>75</v>
       </c>
       <c r="N78" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="O78" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="P78" s="6" t="s">
-        <v>384</v>
+        <v>361</v>
       </c>
       <c r="Q78" s="17"/>
       <c r="R78" s="17">
@@ -5647,20 +5655,24 @@
       </c>
       <c r="C79" s="29"/>
       <c r="D79" s="29"/>
-      <c r="I79" t="s">
-        <v>490</v>
-      </c>
+      <c r="G79" s="58" t="s">
+        <v>497</v>
+      </c>
+      <c r="H79" s="58"/>
+      <c r="I79" s="58"/>
+      <c r="J79" s="58"/>
+      <c r="K79" s="58"/>
       <c r="M79" s="4">
         <v>76</v>
       </c>
       <c r="N79" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O79" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="P79" s="6" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
       <c r="Q79" s="17"/>
       <c r="R79" s="17">
@@ -5682,20 +5694,24 @@
         <v>4</v>
       </c>
       <c r="D80" s="29"/>
-      <c r="I80" t="s">
-        <v>491</v>
-      </c>
+      <c r="G80" s="57" t="s">
+        <v>496</v>
+      </c>
+      <c r="H80" s="57"/>
+      <c r="I80" s="57"/>
+      <c r="J80" s="57"/>
+      <c r="K80" s="57"/>
       <c r="M80" s="4">
         <v>77</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="O80" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="P80" s="6" t="s">
-        <v>386</v>
+        <v>363</v>
       </c>
       <c r="Q80" s="17"/>
       <c r="R80" s="17">
@@ -5717,12 +5733,15 @@
         <v>5</v>
       </c>
       <c r="D81" s="29"/>
+      <c r="I81" s="59" t="s">
+        <v>494</v>
+      </c>
       <c r="M81" s="4">
         <v>78</v>
       </c>
       <c r="N81" s="4"/>
       <c r="O81" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P81" s="4"/>
       <c r="Q81" s="17"/>
@@ -5743,14 +5762,17 @@
       </c>
       <c r="C82" s="29"/>
       <c r="D82" s="29"/>
+      <c r="I82" s="56" t="s">
+        <v>495</v>
+      </c>
       <c r="M82" s="4">
         <v>79</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="O82" s="4" t="s">
-        <v>413</v>
+        <v>390</v>
       </c>
       <c r="P82" s="4"/>
       <c r="Q82" s="17"/>
@@ -5782,7 +5804,7 @@
         <v>203</v>
       </c>
       <c r="O83" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="P83" s="4"/>
       <c r="Q83" s="17"/>
@@ -5860,7 +5882,7 @@
         <v>35</v>
       </c>
       <c r="O87" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="P87" s="1"/>
       <c r="Q87" s="15"/>
@@ -5892,45 +5914,45 @@
         <v>34</v>
       </c>
       <c r="O89" t="s">
-        <v>378</v>
+        <v>355</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N90" t="s">
-        <v>414</v>
+        <v>391</v>
       </c>
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C91" s="27" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
       <c r="N91" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O91" t="s">
-        <v>415</v>
+        <v>392</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
       <c r="N92" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O92" t="s">
-        <v>416</v>
+        <v>393</v>
       </c>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
-        <v>391</v>
+        <v>368</v>
       </c>
       <c r="N93" t="s">
-        <v>413</v>
+        <v>390</v>
       </c>
       <c r="O93" t="s">
-        <v>417</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update & more DC-DC modules info
</commit_message>
<xml_diff>
--- a/pin_map.xlsx
+++ b/pin_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="511">
   <si>
     <t>function</t>
   </si>
@@ -126,9 +126,6 @@
     <t>EEPROM</t>
   </si>
   <si>
-    <t>FLASH</t>
-  </si>
-  <si>
     <t>BTN</t>
   </si>
   <si>
@@ -666,9 +663,6 @@
     <t>TMOT, TPS sensor Gnd</t>
   </si>
   <si>
-    <t>Lambda Sensor In</t>
-  </si>
-  <si>
     <t>Knock Sensor (+)</t>
   </si>
   <si>
@@ -729,9 +723,6 @@
     <t>Reserve (fuel level gnd)</t>
   </si>
   <si>
-    <t>A/C Kompressor Switch</t>
-  </si>
-  <si>
     <t>Vehicle speed</t>
   </si>
   <si>
@@ -774,9 +765,6 @@
     <t>Clutch switch (in?)</t>
   </si>
   <si>
-    <t>Phase Sensor Input</t>
-  </si>
-  <si>
     <t>GND</t>
   </si>
   <si>
@@ -786,9 +774,6 @@
     <t>OUT5</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>OUT12_LOW</t>
   </si>
   <si>
@@ -858,9 +843,6 @@
     <t>OEM function</t>
   </si>
   <si>
-    <t>not used</t>
-  </si>
-  <si>
     <t>fast-power-out (8110)</t>
   </si>
   <si>
@@ -1098,18 +1080,6 @@
     <t>MAP4</t>
   </si>
   <si>
-    <t>ION1</t>
-  </si>
-  <si>
-    <t>ION2</t>
-  </si>
-  <si>
-    <t>ION3</t>
-  </si>
-  <si>
-    <t>ION4</t>
-  </si>
-  <si>
     <t>0*</t>
   </si>
   <si>
@@ -1431,9 +1401,6 @@
     <t>MAP/MAF sensor Gnd</t>
   </si>
   <si>
-    <t>Lambda Sensor 2 In</t>
-  </si>
-  <si>
     <t>SPI0_SOUT/ADC0_5/UART0_TX</t>
   </si>
   <si>
@@ -1510,6 +1477,78 @@
   </si>
   <si>
     <t>*The yellow are non-remappable pins (no suitable options)</t>
+  </si>
+  <si>
+    <t>Lambda Sensor In (O2S)</t>
+  </si>
+  <si>
+    <t>Cam/Phase Sensor Input</t>
+  </si>
+  <si>
+    <t>PPS</t>
+  </si>
+  <si>
+    <t>EGT</t>
+  </si>
+  <si>
+    <t>V12_PERM</t>
+  </si>
+  <si>
+    <t>TPS</t>
+  </si>
+  <si>
+    <t>O2S</t>
+  </si>
+  <si>
+    <t>Lambda Sensor 2 In (O2S_2)</t>
+  </si>
+  <si>
+    <t>AUX_TRIG1</t>
+  </si>
+  <si>
+    <t>AUX_TRIG2</t>
+  </si>
+  <si>
+    <t>AUX_TRIG3</t>
+  </si>
+  <si>
+    <t>AUX_TRIG4</t>
+  </si>
+  <si>
+    <t>CAM</t>
+  </si>
+  <si>
+    <t>LIN</t>
+  </si>
+  <si>
+    <t>Knock</t>
+  </si>
+  <si>
+    <t>Reserved_In2</t>
+  </si>
+  <si>
+    <t>Reserved_In1 / A/C (Bosch)</t>
+  </si>
+  <si>
+    <t>IN (CAM)</t>
+  </si>
+  <si>
+    <t>IN (VSS)</t>
+  </si>
+  <si>
+    <t>IN (TPS)</t>
+  </si>
+  <si>
+    <t>IN O2S)</t>
+  </si>
+  <si>
+    <t>IN (CLT)</t>
+  </si>
+  <si>
+    <t>IN (IAT)</t>
+  </si>
+  <si>
+    <t>(3)</t>
   </si>
 </sst>
 </file>
@@ -1737,7 +1776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1811,6 +1850,12 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1829,11 +1874,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2184,7 +2227,7 @@
   <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,170 +2243,170 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="41" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="38" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="38" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="38" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="38" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="38" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="38" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="39" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>481</v>
+        <v>470</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D14" s="38" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D15" s="39" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F16" s="38" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F17" s="38" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F18" s="38" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F19" s="39" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -2372,15 +2415,15 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="35" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="C22" s="45"/>
       <c r="D22" s="35" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="E22" s="45"/>
       <c r="F22" s="35" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -2401,15 +2444,15 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="35" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="C24" s="45"/>
       <c r="D24" s="35" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="E24" s="45"/>
       <c r="F24" s="35" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -2433,8 +2476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2460,41 +2503,41 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="57" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="G2" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="G2" s="51" t="s">
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="M2" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="M2" s="51" t="s">
-        <v>200</v>
-      </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
       <c r="Q2" s="21"/>
-      <c r="R2" s="52" t="s">
-        <v>199</v>
-      </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="49" t="s">
-        <v>354</v>
-      </c>
-      <c r="V2" s="50"/>
+      <c r="R2" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="S2" s="59"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="55" t="s">
+        <v>348</v>
+      </c>
+      <c r="V2" s="56"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>0</v>
@@ -2503,10 +2546,10 @@
         <v>29</v>
       </c>
       <c r="G3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>0</v>
@@ -2515,26 +2558,26 @@
         <v>29</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="O3" s="10" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="Q3" s="22"/>
       <c r="R3" s="22" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="S3" s="23" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="T3" s="23" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="U3" s="23">
         <v>8110</v>
@@ -2545,33 +2588,33 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="47" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D4" s="43"/>
       <c r="G4" s="4">
         <v>1</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="M4" s="4">
         <v>1</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="P4" s="12"/>
       <c r="Q4" s="24"/>
@@ -2585,33 +2628,33 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="47" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D5" s="43"/>
       <c r="G5" s="4">
         <v>2</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="M5" s="4">
         <v>2</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="25"/>
@@ -2625,33 +2668,33 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="47" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="D6" s="43"/>
       <c r="G6" s="4">
         <v>3</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="M6" s="4">
         <v>3</v>
       </c>
       <c r="N6" s="28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="25"/>
@@ -2663,33 +2706,33 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="B7" s="43"/>
       <c r="C7" s="48" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="D7" s="43"/>
       <c r="G7" s="4">
         <v>4</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="M7" s="4">
         <v>4</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="25"/>
@@ -2703,11 +2746,11 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="47" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="D8" s="43"/>
       <c r="G8" s="4">
@@ -2715,22 +2758,22 @@
         <v>5</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="M8" s="4">
         <v>5</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="25"/>
@@ -2744,11 +2787,11 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="32" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="D9" s="32"/>
       <c r="G9" s="4">
@@ -2756,119 +2799,119 @@
         <v>6</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="M9" s="4">
         <v>6</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="Q9" s="25"/>
       <c r="R9" s="25"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="V9" s="5"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="G10" s="32">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H10" s="43" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J10" s="46" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="M10" s="4">
         <v>7</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="P10" s="11" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="V10" s="5"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="G11" s="32">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H11" s="43" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="J11" s="46" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="M11" s="4">
         <v>8</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
@@ -2876,46 +2919,46 @@
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="G12" s="32">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H12" s="43" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="I12" s="44" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="J12" s="46" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="M12" s="4">
         <v>9</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="Q12" s="25"/>
       <c r="R12" s="25"/>
@@ -2928,38 +2971,38 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="G13" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="H13" s="43" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="J13" s="44" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="M13" s="4">
         <v>10</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="25"/>
@@ -2968,44 +3011,44 @@
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
       <c r="V13" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="M14" s="4">
         <v>11</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="11" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="P14" s="11" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="Q14" s="25"/>
       <c r="R14" s="25"/>
@@ -3018,42 +3061,40 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="M15" s="4">
         <v>12</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O15" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="P15" s="11" t="s">
-        <v>280</v>
-      </c>
+        <v>491</v>
+      </c>
+      <c r="P15" s="11"/>
       <c r="Q15" s="25"/>
       <c r="R15" s="25"/>
       <c r="S15" s="5"/>
@@ -3063,44 +3104,44 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="M16" s="4">
         <v>13</v>
       </c>
       <c r="N16" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="25"/>
       <c r="R16" s="25"/>
       <c r="S16" s="5" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
@@ -3108,38 +3149,38 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>303</v>
-      </c>
-      <c r="I17" s="55" t="s">
-        <v>484</v>
+        <v>297</v>
+      </c>
+      <c r="I17" s="49" t="s">
+        <v>473</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="M17" s="4">
         <v>14</v>
       </c>
       <c r="N17" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="25"/>
@@ -3153,13 +3194,13 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="D18" s="33" t="s">
         <v>32</v>
@@ -3169,22 +3210,22 @@
         <v>15</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="I18" s="55" t="s">
-        <v>485</v>
+        <v>180</v>
+      </c>
+      <c r="I18" s="49" t="s">
+        <v>474</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="M18" s="4">
         <v>15</v>
       </c>
       <c r="N18" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="25"/>
@@ -3198,13 +3239,13 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="D19" s="33" t="s">
         <v>32</v>
@@ -3214,27 +3255,29 @@
         <v>16</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="M19" s="4">
         <v>16</v>
       </c>
       <c r="N19" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O19" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="P19" s="11"/>
+        <v>254</v>
+      </c>
+      <c r="P19" s="11" t="s">
+        <v>492</v>
+      </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="25"/>
-      <c r="S19" s="5">
+      <c r="S19" s="7">
         <v>1</v>
       </c>
       <c r="T19" s="5"/>
@@ -3243,38 +3286,38 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="M20" s="4">
         <v>17</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="P20" s="12"/>
       <c r="Q20" s="24"/>
@@ -3286,41 +3329,43 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="I21" s="55" t="s">
-        <v>482</v>
+        <v>138</v>
+      </c>
+      <c r="I21" s="49" t="s">
+        <v>471</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="M21" s="4">
         <v>18</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>216</v>
+        <v>487</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="P21" s="11"/>
+        <v>254</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>493</v>
+      </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
-      <c r="S21" s="5">
+      <c r="S21" s="7">
         <v>2</v>
       </c>
       <c r="T21" s="5"/>
@@ -3329,40 +3374,42 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="I22" s="55" t="s">
-        <v>483</v>
+        <v>137</v>
+      </c>
+      <c r="I22" s="49" t="s">
+        <v>472</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="M22" s="4">
         <v>19</v>
       </c>
       <c r="N22" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O22" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="P22" s="11"/>
+        <v>253</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>501</v>
+      </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="25">
         <v>1</v>
@@ -3374,38 +3421,38 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I23" s="20" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>337</v>
+        <v>504</v>
       </c>
       <c r="M23" s="4">
         <v>20</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O23" s="12" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="P23" s="12"/>
       <c r="Q23" s="24"/>
@@ -3417,36 +3464,36 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24" s="32" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>337</v>
+        <v>505</v>
       </c>
       <c r="M24" s="4">
         <v>21</v>
       </c>
       <c r="N24" s="4"/>
       <c r="O24" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="P24" s="12"/>
       <c r="Q24" s="24"/>
@@ -3460,36 +3507,36 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="M25" s="4">
         <v>22</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="P25" s="12"/>
       <c r="Q25" s="24"/>
@@ -3503,38 +3550,38 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="M26" s="4">
         <v>23</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O26" s="11" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="25"/>
@@ -3542,39 +3589,41 @@
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
+      <c r="V26" s="61" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="M27" s="4">
         <v>24</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
@@ -3587,177 +3636,177 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="M28" s="4">
         <v>25</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O28" s="11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="P28" s="11" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="25"/>
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
       <c r="U28" s="5" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="V28" s="5"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="M29" s="4">
         <v>26</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O29" s="11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="P29" s="11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="Q29" s="25"/>
       <c r="R29" s="25"/>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
       <c r="U29" s="5" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="V29" s="5"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>337</v>
+        <v>506</v>
       </c>
       <c r="M30" s="4">
         <v>27</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="O30" s="11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="P30" s="11" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="25"/>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
       <c r="U30" s="5" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="V30" s="5"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>337</v>
+        <v>507</v>
       </c>
       <c r="M31" s="4">
         <v>28</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="O31" s="11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="25"/>
@@ -3766,15 +3815,15 @@
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
       <c r="V31" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -3783,25 +3832,25 @@
         <v>29</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>337</v>
+        <v>508</v>
       </c>
       <c r="M32" s="4">
         <v>29</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="O32" s="11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P32" s="11" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="25"/>
@@ -3809,34 +3858,34 @@
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
       <c r="V32" s="5" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="G33" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>337</v>
+        <v>509</v>
       </c>
       <c r="M33" s="4">
         <v>30</v>
@@ -3852,37 +3901,35 @@
       <c r="V33" s="5"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="31" t="s">
-        <v>36</v>
-      </c>
+      <c r="A34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="54"/>
       <c r="G34" s="4">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I34" s="20" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="M34" s="4">
         <v>31</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O34" s="11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P34" s="11"/>
       <c r="Q34" s="25"/>
@@ -3891,43 +3938,43 @@
       <c r="T34" s="5"/>
       <c r="U34" s="5"/>
       <c r="V34" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="M35" s="4">
         <v>32</v>
       </c>
       <c r="N35" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O35" s="11" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="P35" s="11"/>
       <c r="Q35" s="25"/>
@@ -3939,10 +3986,10 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C36" s="44" t="s">
         <v>26</v>
@@ -3955,22 +4002,22 @@
         <v>33</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I36" s="20" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="M36" s="4">
         <v>33</v>
       </c>
       <c r="N36" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O36" s="11" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="P36" s="11"/>
       <c r="Q36" s="25"/>
@@ -3982,10 +4029,10 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -3994,22 +4041,22 @@
         <v>34</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I37" s="20" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="M37" s="4">
         <v>34</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="O37" s="11" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="P37" s="11"/>
       <c r="Q37" s="25"/>
@@ -4021,10 +4068,10 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -4033,22 +4080,22 @@
         <v>35</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="M38" s="4">
         <v>35</v>
       </c>
       <c r="N38" s="28" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="O38" s="11" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="P38" s="11"/>
       <c r="Q38" s="25"/>
@@ -4060,10 +4107,10 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -4072,22 +4119,22 @@
         <v>36</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="M39" s="4">
         <v>36</v>
       </c>
       <c r="N39" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="O39" s="11" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="P39" s="11"/>
       <c r="Q39" s="25"/>
@@ -4099,10 +4146,10 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -4111,25 +4158,25 @@
         <v>37</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="M40" s="4">
         <v>37</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="O40" s="11" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="P40" s="12" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="Q40" s="25"/>
       <c r="R40" s="25"/>
@@ -4142,39 +4189,39 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I41" s="20" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="M41" s="4">
         <v>38</v>
       </c>
       <c r="N41" s="4"/>
       <c r="O41" s="11" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="P41" s="12" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="Q41" s="25"/>
       <c r="R41" s="25"/>
@@ -4187,38 +4234,38 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I42" s="20" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="M42" s="4">
         <v>39</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O42" s="11" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="P42" s="11"/>
       <c r="Q42" s="25"/>
@@ -4232,38 +4279,38 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="G43" s="32">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="H43" s="43" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="I43" s="44" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="J43" s="44" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="M43" s="4">
         <v>40</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="O43" s="11" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="P43" s="11"/>
       <c r="Q43" s="25"/>
@@ -4277,39 +4324,39 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="G44" s="32">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="H44" s="43" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="I44" s="44" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="J44" s="44" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="M44" s="4">
         <v>41</v>
       </c>
       <c r="N44" s="4"/>
       <c r="O44" s="11" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="P44" s="12" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="Q44" s="25"/>
       <c r="R44" s="25"/>
@@ -4322,41 +4369,41 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="M45" s="4">
         <v>42</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="O45" s="11" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="P45" s="12" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="25"/>
@@ -4369,29 +4416,29 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="M46" s="4">
         <v>43</v>
@@ -4408,38 +4455,38 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="G47" s="4">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="J47" s="11" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="M47" s="4">
         <v>44</v>
       </c>
       <c r="N47" s="19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O47" s="11" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="P47" s="11"/>
       <c r="Q47" s="25"/>
@@ -4451,38 +4498,38 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="G48" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="M48" s="4">
         <v>45</v>
       </c>
       <c r="N48" s="19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O48" s="11" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="P48" s="11"/>
       <c r="Q48" s="25"/>
@@ -4494,38 +4541,38 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="G49" s="4">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I49" s="20" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="M49" s="4">
         <v>46</v>
       </c>
       <c r="N49" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="O49" s="11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P49" s="11"/>
       <c r="Q49" s="25"/>
@@ -4539,13 +4586,13 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="D50" s="4"/>
       <c r="G50" s="4">
@@ -4553,69 +4600,67 @@
         <v>47</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="M50" s="4">
         <v>47</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="O50" s="11" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="P50" s="11" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="Q50" s="25"/>
       <c r="R50" s="25"/>
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
       <c r="U50" s="5" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="V50" s="5"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A51" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" s="43" t="s">
-        <v>148</v>
-      </c>
-      <c r="C51" s="32" t="s">
+      <c r="A51" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="31" t="s">
-        <v>36</v>
-      </c>
+      <c r="D51" s="54"/>
       <c r="G51" s="4">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="M51" s="4">
         <v>48</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="O51" s="11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P51" s="11"/>
       <c r="Q51" s="25"/>
@@ -4629,29 +4674,29 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="G52" s="4">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I52" s="20" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="M52" s="4">
         <v>49</v>
@@ -4668,38 +4713,38 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="G53" s="4">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I53" s="20" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="M53" s="4">
         <v>50</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="O53" s="11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P53" s="11"/>
       <c r="Q53" s="25"/>
@@ -4713,38 +4758,38 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="G54" s="4">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="M54" s="4">
         <v>51</v>
       </c>
       <c r="N54" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O54" s="11" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="P54" s="11"/>
       <c r="Q54" s="25"/>
@@ -4756,38 +4801,40 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="G55" s="4">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="M55" s="4">
         <v>52</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
+      <c r="P55" s="11" t="s">
+        <v>500</v>
+      </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="25"/>
       <c r="S55" s="5"/>
@@ -4797,38 +4844,38 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="G56" s="4">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I56" s="20" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="M56" s="4">
         <v>53</v>
       </c>
       <c r="N56" s="28" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O56" s="11" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="P56" s="11"/>
       <c r="Q56" s="25"/>
@@ -4840,29 +4887,29 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="G57" s="4">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="J57" s="11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="M57" s="4">
         <v>54</v>
@@ -4879,38 +4926,38 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="G58" s="4">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="M58" s="4">
         <v>55</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>471</v>
+        <v>494</v>
       </c>
       <c r="O58" s="11" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="P58" s="11"/>
       <c r="Q58" s="25"/>
@@ -4924,39 +4971,39 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="G59" s="4">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="J59" s="11" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="M59" s="4">
         <v>56</v>
       </c>
       <c r="N59" s="4"/>
       <c r="O59" s="11" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="P59" s="11" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="Q59" s="25"/>
       <c r="R59" s="25"/>
@@ -4967,10 +5014,10 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C60" s="29"/>
       <c r="D60" s="29" t="s">
@@ -4981,20 +5028,20 @@
         <v>57</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I60" s="20" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="J60" s="11" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="M60" s="4">
         <v>57</v>
       </c>
       <c r="N60" s="4"/>
       <c r="O60" s="11" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="P60" s="11"/>
       <c r="Q60" s="25"/>
@@ -5006,10 +5053,10 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C61" s="29" t="s">
         <v>19</v>
@@ -5020,24 +5067,26 @@
         <v>58</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I61" s="20" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="J61" s="11" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="M61" s="4">
         <v>58</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>237</v>
+        <v>503</v>
       </c>
       <c r="O61" s="11" t="s">
-        <v>390</v>
-      </c>
-      <c r="P61" s="11"/>
+        <v>380</v>
+      </c>
+      <c r="P61" s="11" t="s">
+        <v>490</v>
+      </c>
       <c r="Q61" s="25"/>
       <c r="R61" s="25"/>
       <c r="S61" s="5">
@@ -5049,10 +5098,10 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C62" s="29"/>
       <c r="D62" s="29" t="s">
@@ -5063,24 +5112,26 @@
         <v>59</v>
       </c>
       <c r="H62" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="I62" s="55" t="s">
-        <v>478</v>
+        <v>182</v>
+      </c>
+      <c r="I62" s="49" t="s">
+        <v>467</v>
       </c>
       <c r="J62" s="11" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="M62" s="4">
         <v>59</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O62" s="11" t="s">
-        <v>390</v>
-      </c>
-      <c r="P62" s="11"/>
+        <v>380</v>
+      </c>
+      <c r="P62" s="11" t="s">
+        <v>312</v>
+      </c>
       <c r="Q62" s="25"/>
       <c r="R62" s="25"/>
       <c r="S62" s="5">
@@ -5092,10 +5143,10 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C63" s="29" t="s">
         <v>20</v>
@@ -5106,13 +5157,13 @@
         <v>60</v>
       </c>
       <c r="H63" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="I63" s="55" t="s">
-        <v>479</v>
+        <v>181</v>
+      </c>
+      <c r="I63" s="49" t="s">
+        <v>468</v>
       </c>
       <c r="J63" s="11" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="M63" s="4">
         <v>60</v>
@@ -5129,10 +5180,10 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C64" s="29" t="s">
         <v>8</v>
@@ -5143,22 +5194,22 @@
         <v>61</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I64" s="11" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="J64" s="11" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="M64" s="4">
         <v>61</v>
       </c>
       <c r="N64" s="28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O64" s="11" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="P64" s="11"/>
       <c r="Q64" s="25"/>
@@ -5170,10 +5221,10 @@
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C65" s="29"/>
       <c r="D65" s="31" t="s">
@@ -5184,13 +5235,13 @@
         <v>62</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="J65" s="11" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="M65" s="4">
         <v>62</v>
@@ -5207,13 +5258,13 @@
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D66" s="33" t="s">
         <v>30</v>
@@ -5223,22 +5274,22 @@
         <v>63</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I66" s="20" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="J66" s="11" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="M66" s="4">
         <v>63</v>
       </c>
       <c r="N66" s="28" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O66" s="11" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="P66" s="11"/>
       <c r="Q66" s="25"/>
@@ -5250,10 +5301,10 @@
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C67" s="29" t="s">
         <v>9</v>
@@ -5264,25 +5315,25 @@
         <v>64</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="J67" s="11" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="M67" s="4">
         <v>64</v>
       </c>
       <c r="N67" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="O67" s="11" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="P67" s="11" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="Q67" s="25"/>
       <c r="R67" s="25"/>
@@ -5293,10 +5344,10 @@
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C68" s="29" t="s">
         <v>27</v>
@@ -5308,10 +5359,10 @@
         <v>65</v>
       </c>
       <c r="N68" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O68" s="11" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="P68" s="11"/>
       <c r="Q68" s="25"/>
@@ -5323,10 +5374,10 @@
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C69" s="29" t="s">
         <v>11</v>
@@ -5335,16 +5386,16 @@
         <v>31</v>
       </c>
       <c r="I69" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="M69" s="4">
         <v>66</v>
       </c>
       <c r="N69" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O69" s="11" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="P69" s="11"/>
       <c r="Q69" s="25"/>
@@ -5356,10 +5407,10 @@
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C70" s="29"/>
       <c r="D70" s="32"/>
@@ -5367,10 +5418,10 @@
         <v>67</v>
       </c>
       <c r="N70" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="O70" s="11" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="P70" s="11"/>
       <c r="Q70" s="25"/>
@@ -5382,10 +5433,10 @@
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C71" s="29" t="s">
         <v>28</v>
@@ -5394,16 +5445,16 @@
         <v>28</v>
       </c>
       <c r="G71" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="M71" s="4">
         <v>68</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="O71" s="11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P71" s="11"/>
       <c r="Q71" s="25"/>
@@ -5417,10 +5468,10 @@
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C72" s="29" t="s">
         <v>22</v>
@@ -5429,16 +5480,16 @@
         <v>33</v>
       </c>
       <c r="G72" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="M72" s="4">
         <v>69</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="O72" s="13" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P72" s="13"/>
       <c r="Q72" s="26"/>
@@ -5452,10 +5503,10 @@
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C73" s="29" t="s">
         <v>21</v>
@@ -5464,16 +5515,16 @@
         <v>33</v>
       </c>
       <c r="G73" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="M73" s="4">
         <v>70</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="O73" s="4" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="P73" s="4"/>
       <c r="Q73" s="17"/>
@@ -5487,10 +5538,10 @@
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C74" s="29" t="s">
         <v>23</v>
@@ -5499,19 +5550,19 @@
         <v>33</v>
       </c>
       <c r="G74" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="M74" s="4">
         <v>71</v>
       </c>
       <c r="N74" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O74" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="P74" s="4" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="Q74" s="17"/>
       <c r="R74" s="17"/>
@@ -5522,23 +5573,23 @@
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C75" s="29" t="s">
         <v>10</v>
       </c>
       <c r="D75" s="29"/>
       <c r="G75" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="M75" s="4">
         <v>72</v>
       </c>
       <c r="N75" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="O75" s="4"/>
       <c r="P75" s="4"/>
@@ -5551,17 +5602,17 @@
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="29" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C76" s="29" t="s">
         <v>11</v>
       </c>
       <c r="D76" s="29"/>
       <c r="G76" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="M76" s="4">
         <v>73</v>
@@ -5578,10 +5629,10 @@
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C77" s="29" t="s">
         <v>24</v>
@@ -5590,19 +5641,19 @@
         <v>33</v>
       </c>
       <c r="G77" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="M77" s="4">
         <v>74</v>
       </c>
       <c r="N77" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O77" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="P77" s="6" t="s">
-        <v>360</v>
+        <v>495</v>
       </c>
       <c r="Q77" s="17"/>
       <c r="R77" s="17">
@@ -5615,27 +5666,27 @@
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C78" s="29"/>
       <c r="D78" s="29"/>
       <c r="G78" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
       <c r="M78" s="4">
         <v>75</v>
       </c>
       <c r="N78" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="O78" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="P78" s="6" t="s">
-        <v>361</v>
+        <v>496</v>
       </c>
       <c r="Q78" s="17"/>
       <c r="R78" s="17">
@@ -5648,31 +5699,31 @@
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C79" s="29"/>
       <c r="D79" s="29"/>
-      <c r="G79" s="58" t="s">
-        <v>497</v>
-      </c>
-      <c r="H79" s="58"/>
-      <c r="I79" s="58"/>
-      <c r="J79" s="58"/>
-      <c r="K79" s="58"/>
+      <c r="G79" s="52" t="s">
+        <v>486</v>
+      </c>
+      <c r="H79" s="52"/>
+      <c r="I79" s="52"/>
+      <c r="J79" s="52"/>
+      <c r="K79" s="52"/>
       <c r="M79" s="4">
         <v>76</v>
       </c>
       <c r="N79" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="O79" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="P79" s="6" t="s">
-        <v>362</v>
+        <v>497</v>
       </c>
       <c r="Q79" s="17"/>
       <c r="R79" s="17">
@@ -5685,33 +5736,33 @@
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C80" s="29" t="s">
         <v>4</v>
       </c>
       <c r="D80" s="29"/>
-      <c r="G80" s="57" t="s">
-        <v>496</v>
-      </c>
-      <c r="H80" s="57"/>
-      <c r="I80" s="57"/>
-      <c r="J80" s="57"/>
-      <c r="K80" s="57"/>
+      <c r="G80" s="51" t="s">
+        <v>485</v>
+      </c>
+      <c r="H80" s="51"/>
+      <c r="I80" s="51"/>
+      <c r="J80" s="51"/>
+      <c r="K80" s="51"/>
       <c r="M80" s="4">
         <v>77</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="O80" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="P80" s="6" t="s">
-        <v>363</v>
+        <v>498</v>
       </c>
       <c r="Q80" s="17"/>
       <c r="R80" s="17">
@@ -5724,26 +5775,30 @@
     </row>
     <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B81" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C81" s="29" t="s">
         <v>5</v>
       </c>
       <c r="D81" s="29"/>
-      <c r="I81" s="59" t="s">
-        <v>494</v>
+      <c r="I81" s="53" t="s">
+        <v>483</v>
       </c>
       <c r="M81" s="4">
         <v>78</v>
       </c>
-      <c r="N81" s="4"/>
+      <c r="N81" s="4" t="s">
+        <v>502</v>
+      </c>
       <c r="O81" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="P81" s="4"/>
+        <v>254</v>
+      </c>
+      <c r="P81" s="4" t="s">
+        <v>489</v>
+      </c>
       <c r="Q81" s="17"/>
       <c r="R81" s="17"/>
       <c r="S81" s="5">
@@ -5755,26 +5810,28 @@
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C82" s="29"/>
       <c r="D82" s="29"/>
-      <c r="I82" s="56" t="s">
-        <v>495</v>
+      <c r="I82" s="50" t="s">
+        <v>484</v>
       </c>
       <c r="M82" s="4">
         <v>79</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>252</v>
+        <v>488</v>
       </c>
       <c r="O82" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="P82" s="4"/>
+        <v>380</v>
+      </c>
+      <c r="P82" s="4" t="s">
+        <v>499</v>
+      </c>
       <c r="Q82" s="17"/>
       <c r="R82" s="17"/>
       <c r="S82" s="5">
@@ -5786,25 +5843,23 @@
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B83" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C83" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D83" s="34" t="s">
-        <v>36</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D83" s="34"/>
       <c r="M83" s="4">
         <v>80</v>
       </c>
       <c r="N83" s="28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O83" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="P83" s="4"/>
       <c r="Q83" s="17"/>
@@ -5816,17 +5871,15 @@
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B84" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C84" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D84" s="34" t="s">
-        <v>36</v>
-      </c>
+      <c r="D84" s="34"/>
       <c r="M84" s="5">
         <v>81</v>
       </c>
@@ -5842,47 +5895,45 @@
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A85" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C85" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D85" s="34" t="s">
-        <v>36</v>
-      </c>
+      <c r="D85" s="34"/>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A86" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C86" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D86" s="34" t="s">
+      <c r="D86" s="31" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A87" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C87" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D87" s="34" t="s">
+      <c r="D87" s="31" t="s">
         <v>35</v>
       </c>
       <c r="O87" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="P87" s="1"/>
       <c r="Q87" s="15"/>
@@ -5890,10 +5941,10 @@
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C88" s="29" t="s">
         <v>10</v>
@@ -5902,10 +5953,10 @@
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A89" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C89" s="29" t="s">
         <v>11</v>
@@ -5914,45 +5965,45 @@
         <v>34</v>
       </c>
       <c r="O89" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N90" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="91" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C91" s="27" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="N91" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="O91" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="N92" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="O92" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="N93" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="O93" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pcb progress: 30% complete
</commit_message>
<xml_diff>
--- a/pin_map.xlsx
+++ b/pin_map.xlsx
@@ -2635,7 +2635,7 @@
   <dimension ref="A2:W93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3787,7 +3787,7 @@
         <v>286</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M28" s="4">
         <v>25</v>
@@ -3833,7 +3833,7 @@
         <v>287</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M29" s="4">
         <v>26</v>
@@ -4320,7 +4320,7 @@
         <v>296</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M40" s="4">
         <v>37</v>
@@ -4628,7 +4628,7 @@
         <v>301</v>
       </c>
       <c r="J47" s="11" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M47" s="4">
         <v>44</v>

</xml_diff>

<commit_message>
add compatibility with Mikas 10.3
</commit_message>
<xml_diff>
--- a/pin_map.xlsx
+++ b/pin_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="569">
   <si>
     <t>function</t>
   </si>
@@ -792,9 +792,6 @@
     <t>K-LINE</t>
   </si>
   <si>
-    <t>HOT Lamp / Starter Relay 2</t>
-  </si>
-  <si>
     <t>comments</t>
   </si>
   <si>
@@ -1515,18 +1512,12 @@
     <t>Reserve (out) / Idle-hyundai1</t>
   </si>
   <si>
-    <t>ECF Relay 2  / Idle-hyundai2</t>
-  </si>
-  <si>
     <t>(=3)</t>
   </si>
   <si>
     <t>*lada-priora fans?</t>
   </si>
   <si>
-    <t>used as idle-pwm in hyundai accent</t>
-  </si>
-  <si>
     <t>used as idle pwm in hyundai accent</t>
   </si>
   <si>
@@ -1575,9 +1566,6 @@
     <t>*MODULE4</t>
   </si>
   <si>
-    <t>*MODULE5</t>
-  </si>
-  <si>
     <t>*MODULE6</t>
   </si>
   <si>
@@ -1635,9 +1623,6 @@
     <t>Reserved_In2 / AC (Bosch)</t>
   </si>
   <si>
-    <t>GPIO (EXTI6)</t>
-  </si>
-  <si>
     <t>UTX4 (EXTI0)</t>
   </si>
   <si>
@@ -1714,6 +1699,30 @@
   </si>
   <si>
     <t>GPIO/SWD_DIO</t>
+  </si>
+  <si>
+    <t>GPIO (EXTI3)</t>
+  </si>
+  <si>
+    <t>*MODULE5 / MAP (mikas)</t>
+  </si>
+  <si>
+    <t>ECF Relay 2  / Idle2 (hyundai/mikas)</t>
+  </si>
+  <si>
+    <t>HOTLamp / Starter Relay / Idle1(Mikas)</t>
+  </si>
+  <si>
+    <t>* used for Idle in Mikas 10.3</t>
+  </si>
+  <si>
+    <t>used as idle-pwm in hyundai accent and Mikas 10.3</t>
+  </si>
+  <si>
+    <t>* connected to pin #56 in Mikas config</t>
+  </si>
+  <si>
+    <t>* for Mikas config, connected to pin #38</t>
   </si>
 </sst>
 </file>
@@ -2401,170 +2410,170 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="41" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="D2" s="41" t="s">
-        <v>272</v>
-      </c>
       <c r="F2" s="41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="38" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="38" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="38" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="38" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="38" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="38" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="39" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D14" s="38" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D15" s="39" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F16" s="38" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F17" s="38" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F18" s="38" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F19" s="39" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -2573,15 +2582,15 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C22" s="45"/>
       <c r="D22" s="35" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E22" s="45"/>
       <c r="F22" s="35" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -2602,15 +2611,15 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="35" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C24" s="45"/>
       <c r="D24" s="35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E24" s="45"/>
       <c r="F24" s="35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -2634,8 +2643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="W59" sqref="W59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2653,7 +2662,7 @@
     <col min="11" max="11" width="5.140625" customWidth="1"/>
     <col min="12" max="12" width="3.28515625" customWidth="1"/>
     <col min="13" max="13" width="5.5703125" customWidth="1"/>
-    <col min="14" max="14" width="29.140625" customWidth="1"/>
+    <col min="14" max="14" width="36.140625" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" customWidth="1"/>
     <col min="16" max="16" width="26.140625" customWidth="1"/>
     <col min="17" max="18" width="3.28515625" style="16" customWidth="1"/>
@@ -2686,7 +2695,7 @@
       <c r="S2" s="57"/>
       <c r="T2" s="58"/>
       <c r="U2" s="54" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -2718,23 +2727,23 @@
         <v>112</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O3" s="10" t="s">
         <v>27</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q3" s="22"/>
       <c r="R3" s="22" t="s">
+        <v>324</v>
+      </c>
+      <c r="S3" s="23" t="s">
         <v>325</v>
       </c>
-      <c r="S3" s="23" t="s">
+      <c r="T3" s="23" t="s">
         <v>326</v>
-      </c>
-      <c r="T3" s="23" t="s">
-        <v>327</v>
       </c>
       <c r="U3" s="54">
         <v>6240</v>
@@ -2742,7 +2751,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="47" t="s">
@@ -2756,10 +2765,10 @@
         <v>163</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M4" s="4">
         <v>1</v>
@@ -2768,7 +2777,7 @@
         <v>197</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P4" s="12"/>
       <c r="Q4" s="24"/>
@@ -2781,7 +2790,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="47" t="s">
@@ -2795,10 +2804,10 @@
         <v>162</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M5" s="4">
         <v>2</v>
@@ -2807,7 +2816,7 @@
         <v>198</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="25"/>
@@ -2820,11 +2829,11 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="47" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D6" s="43"/>
       <c r="G6" s="4">
@@ -2834,10 +2843,10 @@
         <v>189</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M6" s="4">
         <v>3</v>
@@ -2846,7 +2855,7 @@
         <v>199</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="25"/>
@@ -2857,11 +2866,11 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B7" s="43"/>
       <c r="C7" s="48" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D7" s="43"/>
       <c r="G7" s="4">
@@ -2871,10 +2880,10 @@
         <v>188</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M7" s="4">
         <v>4</v>
@@ -2883,7 +2892,7 @@
         <v>200</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="25"/>
@@ -2896,11 +2905,11 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="47" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D8" s="43"/>
       <c r="G8" s="4">
@@ -2911,10 +2920,10 @@
         <v>183</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="M8" s="4">
         <v>5</v>
@@ -2923,7 +2932,7 @@
         <v>201</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="25"/>
@@ -2936,11 +2945,11 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="32" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D9" s="32"/>
       <c r="G9" s="4">
@@ -2951,10 +2960,10 @@
         <v>182</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="M9" s="4">
         <v>6</v>
@@ -2963,10 +2972,10 @@
         <v>202</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="Q9" s="25"/>
       <c r="R9" s="25"/>
@@ -2978,29 +2987,29 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>178</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="G10" s="32">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H10" s="43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J10" s="46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M10" s="4">
         <v>7</v>
@@ -3009,10 +3018,10 @@
         <v>203</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="P10" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
@@ -3024,29 +3033,29 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>179</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="G11" s="32">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H11" s="43" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J11" s="46" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M11" s="4">
         <v>8</v>
@@ -3058,7 +3067,7 @@
         <v>246</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
@@ -3070,39 +3079,39 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>180</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="G12" s="32">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H12" s="43" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I12" s="44" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J12" s="46" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M12" s="4">
         <v>9</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="12" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="Q12" s="25"/>
       <c r="R12" s="25"/>
@@ -3118,23 +3127,23 @@
         <v>181</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>426</v>
+        <v>561</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="G13" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="H13" s="43" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J13" s="44" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M13" s="4">
         <v>10</v>
@@ -3162,10 +3171,10 @@
         <v>182</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="0"/>
@@ -3175,10 +3184,10 @@
         <v>137</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="M14" s="4">
         <v>11</v>
@@ -3193,10 +3202,10 @@
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
       <c r="U14" s="5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="W14" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -3207,10 +3216,10 @@
         <v>183</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="0"/>
@@ -3220,10 +3229,10 @@
         <v>136</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M15" s="4">
         <v>12</v>
@@ -3232,7 +3241,7 @@
         <v>206</v>
       </c>
       <c r="O15" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="25"/>
@@ -3249,10 +3258,10 @@
         <v>184</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>539</v>
+        <v>425</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" si="0"/>
@@ -3262,10 +3271,10 @@
         <v>181</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M16" s="4">
         <v>13</v>
@@ -3274,13 +3283,13 @@
         <v>207</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="25"/>
       <c r="R16" s="25"/>
       <c r="S16" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
@@ -3293,7 +3302,7 @@
         <v>159</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D17" s="4"/>
       <c r="G17" s="4">
@@ -3301,13 +3310,13 @@
         <v>14</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I17" s="49" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M17" s="4">
         <v>14</v>
@@ -3335,7 +3344,7 @@
         <v>160</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D18" s="33" t="s">
         <v>30</v>
@@ -3348,10 +3357,10 @@
         <v>177</v>
       </c>
       <c r="I18" s="49" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M18" s="4">
         <v>15</v>
@@ -3379,7 +3388,7 @@
         <v>161</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D19" s="33" t="s">
         <v>30</v>
@@ -3392,10 +3401,10 @@
         <v>187</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M19" s="4">
         <v>16</v>
@@ -3407,7 +3416,7 @@
         <v>248</v>
       </c>
       <c r="P19" s="11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="25"/>
@@ -3425,10 +3434,10 @@
         <v>146</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="0"/>
@@ -3438,10 +3447,10 @@
         <v>186</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M20" s="4">
         <v>17</v>
@@ -3450,7 +3459,7 @@
         <v>211</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P20" s="12"/>
       <c r="Q20" s="24"/>
@@ -3468,7 +3477,7 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="0"/>
@@ -3478,22 +3487,22 @@
         <v>135</v>
       </c>
       <c r="I21" s="49" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M21" s="4">
         <v>18</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="O21" s="11" t="s">
         <v>248</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
@@ -3514,7 +3523,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="0"/>
@@ -3524,10 +3533,10 @@
         <v>134</v>
       </c>
       <c r="I22" s="49" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M22" s="4">
         <v>19</v>
@@ -3539,7 +3548,7 @@
         <v>247</v>
       </c>
       <c r="P22" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="25">
@@ -3560,7 +3569,7 @@
         <v>16</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="0"/>
@@ -3570,10 +3579,10 @@
         <v>149</v>
       </c>
       <c r="I23" s="20" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="M23" s="4">
         <v>20</v>
@@ -3599,10 +3608,10 @@
         <v>114</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="0"/>
@@ -3612,10 +3621,10 @@
         <v>148</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="M24" s="4">
         <v>21</v>
@@ -3625,7 +3634,7 @@
         <v>245</v>
       </c>
       <c r="P24" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q24" s="24"/>
       <c r="R24" s="24"/>
@@ -3646,7 +3655,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
@@ -3656,10 +3665,10 @@
         <v>169</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M25" s="4">
         <v>22</v>
@@ -3669,7 +3678,7 @@
         <v>245</v>
       </c>
       <c r="P25" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q25" s="24"/>
       <c r="R25" s="24"/>
@@ -3687,10 +3696,10 @@
         <v>115</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="0"/>
@@ -3700,19 +3709,19 @@
         <v>168</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M26" s="4">
         <v>23</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="O26" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="25"/>
@@ -3720,7 +3729,7 @@
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
       <c r="U26" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
@@ -3734,7 +3743,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="0"/>
@@ -3744,20 +3753,20 @@
         <v>167</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M27" s="4">
         <v>24</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="O27" s="12"/>
       <c r="P27" s="12" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="Q27" s="24"/>
       <c r="R27" s="24"/>
@@ -3774,7 +3783,7 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="0"/>
@@ -3784,10 +3793,10 @@
         <v>147</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M28" s="4">
         <v>25</v>
@@ -3799,14 +3808,14 @@
         <v>246</v>
       </c>
       <c r="P28" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="25"/>
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
       <c r="U28" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
@@ -3820,7 +3829,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="0"/>
@@ -3830,16 +3839,16 @@
         <v>146</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M29" s="4">
         <v>26</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="O29" s="11" t="s">
         <v>244</v>
@@ -3850,10 +3859,10 @@
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
       <c r="U29" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="W29" t="s">
         <v>500</v>
-      </c>
-      <c r="W29" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
@@ -3867,20 +3876,20 @@
         <v>4</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="H30" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="I30" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="I30" s="11" t="s">
-        <v>289</v>
-      </c>
       <c r="J30" s="11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="M30" s="4">
         <v>27</v>
@@ -3889,10 +3898,10 @@
         <v>215</v>
       </c>
       <c r="O30" s="11" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="P30" s="11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="25"/>
@@ -3913,26 +3922,26 @@
         <v>5</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="H31" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="I31" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="I31" s="11" t="s">
-        <v>291</v>
-      </c>
       <c r="J31" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="M31" s="4">
         <v>28</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O31" s="11" t="s">
         <v>246</v>
@@ -3946,7 +3955,7 @@
         <v>3</v>
       </c>
       <c r="W31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
@@ -3957,10 +3966,10 @@
         <v>150</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G32" s="4">
         <f t="shared" si="0"/>
@@ -3970,22 +3979,22 @@
         <v>161</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M32" s="4">
         <v>29</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>499</v>
+        <v>563</v>
       </c>
       <c r="O32" s="11" t="s">
         <v>246</v>
       </c>
       <c r="P32" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="25"/>
@@ -3995,10 +4004,10 @@
         <v>4</v>
       </c>
       <c r="W32" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>52</v>
       </c>
@@ -4006,10 +4015,10 @@
         <v>151</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G33" s="4">
         <f t="shared" si="0"/>
@@ -4019,10 +4028,10 @@
         <v>160</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="M33" s="4">
         <v>30</v>
@@ -4032,17 +4041,17 @@
         <v>244</v>
       </c>
       <c r="P33" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q33" s="25"/>
       <c r="R33" s="25"/>
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
       <c r="U33" s="5" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>44</v>
       </c>
@@ -4050,10 +4059,10 @@
         <v>130</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="G34" s="4">
         <f t="shared" si="0"/>
@@ -4063,10 +4072,10 @@
         <v>133</v>
       </c>
       <c r="I34" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M34" s="4">
         <v>31</v>
@@ -4086,7 +4095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>45</v>
       </c>
@@ -4094,10 +4103,10 @@
         <v>131</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="0"/>
@@ -4107,10 +4116,10 @@
         <v>132</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M35" s="4">
         <v>32</v>
@@ -4128,7 +4137,7 @@
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
         <v>46</v>
       </c>
@@ -4149,10 +4158,10 @@
         <v>131</v>
       </c>
       <c r="I36" s="20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M36" s="4">
         <v>33</v>
@@ -4170,7 +4179,7 @@
       <c r="T36" s="5"/>
       <c r="U36" s="5"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>60</v>
       </c>
@@ -4178,10 +4187,10 @@
         <v>185</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G37" s="4">
         <f t="shared" si="0"/>
@@ -4191,10 +4200,10 @@
         <v>130</v>
       </c>
       <c r="I37" s="20" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M37" s="4">
         <v>34</v>
@@ -4212,7 +4221,7 @@
       <c r="T37" s="5"/>
       <c r="U37" s="5"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>61</v>
       </c>
@@ -4220,10 +4229,10 @@
         <v>186</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="G38" s="4">
         <f t="shared" si="0"/>
@@ -4233,19 +4242,19 @@
         <v>155</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="M38" s="4">
         <v>35</v>
       </c>
       <c r="N38" s="28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O38" s="11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P38" s="11"/>
       <c r="Q38" s="25"/>
@@ -4254,7 +4263,7 @@
       <c r="T38" s="5"/>
       <c r="U38" s="5"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>62</v>
       </c>
@@ -4262,10 +4271,10 @@
         <v>187</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="G39" s="4">
         <f t="shared" si="0"/>
@@ -4275,10 +4284,10 @@
         <v>154</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="M39" s="4">
         <v>36</v>
@@ -4287,7 +4296,7 @@
         <v>220</v>
       </c>
       <c r="O39" s="11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P39" s="11"/>
       <c r="Q39" s="25"/>
@@ -4296,7 +4305,7 @@
       <c r="T39" s="5"/>
       <c r="U39" s="5"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>64</v>
       </c>
@@ -4304,10 +4313,10 @@
         <v>189</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="G40" s="4">
         <f t="shared" si="0"/>
@@ -4317,22 +4326,22 @@
         <v>121</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M40" s="4">
         <v>37</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="O40" s="11" t="s">
         <v>248</v>
       </c>
       <c r="P40" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q40" s="25"/>
       <c r="R40" s="25"/>
@@ -4342,7 +4351,7 @@
       <c r="T40" s="5"/>
       <c r="U40" s="5"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>63</v>
       </c>
@@ -4350,10 +4359,10 @@
         <v>188</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" si="0"/>
@@ -4363,10 +4372,10 @@
         <v>120</v>
       </c>
       <c r="I41" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M41" s="4">
         <v>38</v>
@@ -4376,7 +4385,7 @@
         <v>248</v>
       </c>
       <c r="P41" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q41" s="25"/>
       <c r="R41" s="25"/>
@@ -4385,8 +4394,11 @@
       </c>
       <c r="T41" s="5"/>
       <c r="U41" s="5"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W41" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>66</v>
       </c>
@@ -4394,10 +4406,10 @@
         <v>191</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="0"/>
@@ -4407,10 +4419,10 @@
         <v>185</v>
       </c>
       <c r="I42" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M42" s="4">
         <v>39</v>
@@ -4430,7 +4442,7 @@
       <c r="T42" s="5"/>
       <c r="U42" s="5"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>65</v>
       </c>
@@ -4438,23 +4450,23 @@
         <v>190</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G43" s="32">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="H43" s="43" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I43" s="44" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J43" s="44" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M43" s="4">
         <v>40</v>
@@ -4474,7 +4486,7 @@
       <c r="T43" s="5"/>
       <c r="U43" s="5"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>68</v>
       </c>
@@ -4482,23 +4494,23 @@
         <v>193</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G44" s="32">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="H44" s="43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I44" s="44" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J44" s="44" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M44" s="4">
         <v>41</v>
@@ -4508,7 +4520,7 @@
         <v>248</v>
       </c>
       <c r="P44" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q44" s="25"/>
       <c r="R44" s="25"/>
@@ -4518,7 +4530,7 @@
       <c r="T44" s="5"/>
       <c r="U44" s="5"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>67</v>
       </c>
@@ -4526,10 +4538,10 @@
         <v>192</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="0"/>
@@ -4539,22 +4551,22 @@
         <v>143</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="M45" s="4">
         <v>42</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O45" s="11" t="s">
         <v>248</v>
       </c>
       <c r="P45" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="25"/>
@@ -4564,7 +4576,7 @@
       <c r="T45" s="5"/>
       <c r="U45" s="5"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>70</v>
       </c>
@@ -4572,10 +4584,10 @@
         <v>141</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" si="0"/>
@@ -4585,10 +4597,10 @@
         <v>142</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J46" s="11" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="M46" s="4">
         <v>43</v>
@@ -4596,7 +4608,7 @@
       <c r="N46" s="8"/>
       <c r="O46" s="11"/>
       <c r="P46" s="12" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="25"/>
@@ -4604,7 +4616,7 @@
       <c r="T46" s="5"/>
       <c r="U46" s="5"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>69</v>
       </c>
@@ -4612,10 +4624,10 @@
         <v>140</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G47" s="4">
         <f t="shared" si="0"/>
@@ -4625,10 +4637,10 @@
         <v>166</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J47" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M47" s="4">
         <v>44</v>
@@ -4646,7 +4658,7 @@
       <c r="T47" s="5"/>
       <c r="U47" s="5"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>72</v>
       </c>
@@ -4654,10 +4666,10 @@
         <v>143</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G48" s="4">
         <f t="shared" si="0"/>
@@ -4667,10 +4679,10 @@
         <v>165</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="M48" s="4">
         <v>45</v>
@@ -4699,7 +4711,7 @@
         <v>14</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G49" s="4">
         <f t="shared" si="0"/>
@@ -4709,10 +4721,10 @@
         <v>164</v>
       </c>
       <c r="I49" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M49" s="4">
         <v>46</v>
@@ -4740,7 +4752,7 @@
         <v>145</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D50" s="4"/>
       <c r="G50" s="4">
@@ -4751,10 +4763,10 @@
         <v>117</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="M50" s="4">
         <v>47</v>
@@ -4763,10 +4775,10 @@
         <v>225</v>
       </c>
       <c r="O50" s="11" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="P50" s="11" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Q50" s="25"/>
       <c r="R50" s="25"/>
@@ -4784,10 +4796,10 @@
         <v>144</v>
       </c>
       <c r="C51" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="D51" s="11" t="s">
         <v>477</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>478</v>
       </c>
       <c r="G51" s="4">
         <f t="shared" si="0"/>
@@ -4797,10 +4809,10 @@
         <v>116</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M51" s="4">
         <v>48</v>
@@ -4831,7 +4843,7 @@
         <v>13</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G52" s="4">
         <f t="shared" si="0"/>
@@ -4841,10 +4853,10 @@
         <v>115</v>
       </c>
       <c r="I52" s="20" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="M52" s="4">
         <v>49</v>
@@ -4859,10 +4871,10 @@
       <c r="S52" s="5"/>
       <c r="T52" s="5"/>
       <c r="U52" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="W52" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
@@ -4876,7 +4888,7 @@
         <v>23</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G53" s="4">
         <f t="shared" si="0"/>
@@ -4886,16 +4898,16 @@
         <v>114</v>
       </c>
       <c r="I53" s="20" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="M53" s="4">
         <v>50</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>258</v>
+        <v>564</v>
       </c>
       <c r="O53" s="11" t="s">
         <v>246</v>
@@ -4908,6 +4920,9 @@
       <c r="U53" s="5">
         <v>7</v>
       </c>
+      <c r="W53" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -4917,10 +4932,10 @@
         <v>173</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G54" s="4">
         <f t="shared" si="0"/>
@@ -4930,10 +4945,10 @@
         <v>153</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="M54" s="4">
         <v>51</v>
@@ -4959,10 +4974,10 @@
         <v>172</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G55" s="4">
         <f t="shared" si="0"/>
@@ -4972,10 +4987,10 @@
         <v>152</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="M55" s="4">
         <v>52</v>
@@ -4985,7 +5000,7 @@
       </c>
       <c r="O55" s="11"/>
       <c r="P55" s="12" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="25"/>
@@ -5001,10 +5016,10 @@
         <v>175</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G56" s="4">
         <f t="shared" si="0"/>
@@ -5014,10 +5029,10 @@
         <v>184</v>
       </c>
       <c r="I56" s="20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M56" s="4">
         <v>53</v>
@@ -5043,7 +5058,7 @@
         <v>174</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D57" s="4"/>
       <c r="G57" s="4">
@@ -5054,20 +5069,20 @@
         <v>180</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J57" s="11" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="M57" s="4">
         <v>54</v>
       </c>
       <c r="N57" s="4"/>
       <c r="O57" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P57" s="11" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Q57" s="25"/>
       <c r="R57" s="25"/>
@@ -5083,10 +5098,10 @@
         <v>177</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="G58" s="4">
         <f t="shared" si="0"/>
@@ -5096,21 +5111,21 @@
         <v>127</v>
       </c>
       <c r="I58" s="20" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M58" s="4">
         <v>55</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O58" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="P58" s="11"/>
+      <c r="P58" s="12"/>
       <c r="Q58" s="25"/>
       <c r="R58" s="25"/>
       <c r="S58" s="5">
@@ -5127,7 +5142,7 @@
         <v>176</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D59" s="4"/>
       <c r="G59" s="4">
@@ -5138,26 +5153,27 @@
         <v>126</v>
       </c>
       <c r="I59" s="20" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="J59" s="11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M59" s="4">
         <v>56</v>
       </c>
       <c r="N59" s="4"/>
-      <c r="O59" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="P59" s="11" t="s">
-        <v>510</v>
+      <c r="O59" s="11"/>
+      <c r="P59" s="12" t="s">
+        <v>562</v>
       </c>
       <c r="Q59" s="25"/>
       <c r="R59" s="25"/>
       <c r="S59" s="5"/>
       <c r="T59" s="5"/>
       <c r="U59" s="5"/>
+      <c r="W59" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="29" t="s">
@@ -5178,18 +5194,20 @@
         <v>125</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J60" s="11" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="M60" s="4">
         <v>57</v>
       </c>
       <c r="N60" s="4"/>
-      <c r="O60" s="11"/>
-      <c r="P60" s="12" t="s">
-        <v>519</v>
+      <c r="O60" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="P60" s="11" t="s">
+        <v>507</v>
       </c>
       <c r="Q60" s="25"/>
       <c r="R60" s="25"/>
@@ -5216,22 +5234,22 @@
         <v>124</v>
       </c>
       <c r="I61" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J61" s="11" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="M61" s="4">
         <v>58</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="O61" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P61" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="Q61" s="25"/>
       <c r="R61" s="25"/>
@@ -5260,10 +5278,10 @@
         <v>179</v>
       </c>
       <c r="I62" s="49" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J62" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M62" s="4">
         <v>59</v>
@@ -5272,10 +5290,10 @@
         <v>229</v>
       </c>
       <c r="O62" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P62" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="Q62" s="25"/>
       <c r="R62" s="25"/>
@@ -5304,10 +5322,10 @@
         <v>178</v>
       </c>
       <c r="I63" s="49" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J63" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M63" s="4">
         <v>60</v>
@@ -5315,7 +5333,7 @@
       <c r="N63" s="4"/>
       <c r="O63" s="11"/>
       <c r="P63" s="12" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="Q63" s="25"/>
       <c r="R63" s="25"/>
@@ -5342,10 +5360,10 @@
         <v>151</v>
       </c>
       <c r="I64" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J64" s="11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M64" s="4">
         <v>61</v>
@@ -5382,10 +5400,10 @@
         <v>150</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="J65" s="11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M65" s="4">
         <v>62</v>
@@ -5393,7 +5411,7 @@
       <c r="N65" s="4"/>
       <c r="O65" s="11"/>
       <c r="P65" s="12" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="Q65" s="25"/>
       <c r="R65" s="25"/>
@@ -5422,10 +5440,10 @@
         <v>119</v>
       </c>
       <c r="I66" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J66" s="11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="M66" s="4">
         <v>63</v>
@@ -5462,10 +5480,10 @@
         <v>118</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="J67" s="11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M67" s="4">
         <v>64</v>
@@ -5477,7 +5495,7 @@
         <v>253</v>
       </c>
       <c r="P67" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Q67" s="25"/>
       <c r="R67" s="25"/>
@@ -5528,7 +5546,7 @@
         <v>29</v>
       </c>
       <c r="I69" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M69" s="4">
         <v>66</v>
@@ -5554,7 +5572,7 @@
         <v>129</v>
       </c>
       <c r="C70" s="29" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="D70" s="32"/>
       <c r="M70" s="4">
@@ -5587,7 +5605,7 @@
         <v>26</v>
       </c>
       <c r="G71" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M71" s="4">
         <v>68</v>
@@ -5621,7 +5639,7 @@
         <v>31</v>
       </c>
       <c r="G72" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M72" s="4">
         <v>69</v>
@@ -5655,7 +5673,7 @@
         <v>31</v>
       </c>
       <c r="G73" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M73" s="4">
         <v>70</v>
@@ -5689,7 +5707,7 @@
         <v>31</v>
       </c>
       <c r="G74" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M74" s="4">
         <v>71</v>
@@ -5701,7 +5719,7 @@
         <v>257</v>
       </c>
       <c r="P74" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Q74" s="17"/>
       <c r="R74" s="17"/>
@@ -5721,7 +5739,7 @@
       </c>
       <c r="D75" s="29"/>
       <c r="G75" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M75" s="4">
         <v>72</v>
@@ -5731,7 +5749,7 @@
       </c>
       <c r="O75" s="4"/>
       <c r="P75" s="12" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="Q75" s="17"/>
       <c r="R75" s="17"/>
@@ -5741,7 +5759,7 @@
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="29" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B76" s="30" t="s">
         <v>163</v>
@@ -5751,7 +5769,7 @@
       </c>
       <c r="D76" s="29"/>
       <c r="G76" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M76" s="4">
         <v>73</v>
@@ -5759,7 +5777,7 @@
       <c r="N76" s="4"/>
       <c r="O76" s="4"/>
       <c r="P76" s="12" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="Q76" s="17"/>
       <c r="R76" s="17"/>
@@ -5781,7 +5799,7 @@
         <v>31</v>
       </c>
       <c r="G77" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="M77" s="4">
         <v>74</v>
@@ -5793,7 +5811,7 @@
         <v>247</v>
       </c>
       <c r="P77" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Q77" s="17"/>
       <c r="R77" s="17">
@@ -5813,7 +5831,7 @@
       <c r="C78" s="29"/>
       <c r="D78" s="29"/>
       <c r="G78" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M78" s="4">
         <v>75</v>
@@ -5825,7 +5843,7 @@
         <v>247</v>
       </c>
       <c r="P78" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="Q78" s="17"/>
       <c r="R78" s="17">
@@ -5845,7 +5863,7 @@
       <c r="C79" s="29"/>
       <c r="D79" s="29"/>
       <c r="G79" s="52" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H79" s="52"/>
       <c r="I79" s="52"/>
@@ -5861,7 +5879,7 @@
         <v>247</v>
       </c>
       <c r="P79" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="Q79" s="17"/>
       <c r="R79" s="17">
@@ -5883,7 +5901,7 @@
       </c>
       <c r="D80" s="29"/>
       <c r="G80" s="51" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H80" s="51"/>
       <c r="I80" s="51"/>
@@ -5899,7 +5917,7 @@
         <v>247</v>
       </c>
       <c r="P80" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="Q80" s="17"/>
       <c r="R80" s="17">
@@ -5921,19 +5939,19 @@
       </c>
       <c r="D81" s="29"/>
       <c r="I81" s="53" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="M81" s="4">
         <v>78</v>
       </c>
       <c r="N81" s="4" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="O81" s="4" t="s">
         <v>248</v>
       </c>
       <c r="P81" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="Q81" s="17"/>
       <c r="R81" s="17"/>
@@ -5953,19 +5971,19 @@
       <c r="C82" s="29"/>
       <c r="D82" s="29"/>
       <c r="I82" s="50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="M82" s="4">
         <v>79</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="O82" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="P82" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Q82" s="17"/>
       <c r="R82" s="17"/>
@@ -6019,7 +6037,7 @@
       <c r="N84" s="4"/>
       <c r="O84" s="4"/>
       <c r="P84" s="12" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="Q84" s="17"/>
       <c r="R84" s="17"/>
@@ -6099,45 +6117,45 @@
         <v>32</v>
       </c>
       <c r="O89" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="N90" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C91" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N91" t="s">
         <v>247</v>
       </c>
       <c r="O91" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="N92" t="s">
         <v>248</v>
       </c>
       <c r="O92" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N93" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="O93" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pcb progress: 60% complete
</commit_message>
<xml_diff>
--- a/pin_map.xlsx
+++ b/pin_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="571">
   <si>
     <t>function</t>
   </si>
@@ -1701,9 +1701,6 @@
     <t>GPIO/SWD_DIO</t>
   </si>
   <si>
-    <t>GPIO (EXTI3)</t>
-  </si>
-  <si>
     <t>*MODULE5 / MAP (mikas)</t>
   </si>
   <si>
@@ -1723,6 +1720,15 @@
   </si>
   <si>
     <t>* for Mikas config, connected to pin #38</t>
+  </si>
+  <si>
+    <t>OUT_TLE6</t>
+  </si>
+  <si>
+    <t>OUT_TLE7</t>
+  </si>
+  <si>
+    <t>GPIO (EXTI2)</t>
   </si>
 </sst>
 </file>
@@ -2643,8 +2649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="W59" sqref="W59"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,7 +3002,7 @@
         <v>425</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>487</v>
+        <v>569</v>
       </c>
       <c r="G10" s="32">
         <f t="shared" si="0"/>
@@ -3042,7 +3048,7 @@
         <v>425</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G11" s="32">
         <f t="shared" si="0"/>
@@ -3085,10 +3091,10 @@
         <v>180</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>425</v>
+        <v>570</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="G12" s="32">
         <f t="shared" si="0"/>
@@ -3127,10 +3133,10 @@
         <v>181</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>561</v>
+        <v>425</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="G13" s="32">
         <f t="shared" si="0"/>
@@ -3174,7 +3180,7 @@
         <v>425</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="0"/>
@@ -3219,7 +3225,7 @@
         <v>425</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="0"/>
@@ -3304,7 +3310,9 @@
       <c r="C17" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>481</v>
+      </c>
       <c r="G17" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3630,18 +3638,14 @@
         <v>21</v>
       </c>
       <c r="N24" s="4"/>
-      <c r="O24" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="P24" s="11" t="s">
-        <v>260</v>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12" t="s">
+        <v>513</v>
       </c>
       <c r="Q24" s="24"/>
       <c r="R24" s="24"/>
       <c r="S24" s="5"/>
-      <c r="T24" s="5">
-        <v>4</v>
-      </c>
+      <c r="T24" s="5"/>
       <c r="U24" s="5"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -3674,18 +3678,14 @@
         <v>22</v>
       </c>
       <c r="N25" s="4"/>
-      <c r="O25" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="P25" s="11" t="s">
-        <v>261</v>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12" t="s">
+        <v>514</v>
       </c>
       <c r="Q25" s="24"/>
       <c r="R25" s="24"/>
       <c r="S25" s="5"/>
-      <c r="T25" s="5">
-        <v>5</v>
-      </c>
+      <c r="T25" s="5"/>
       <c r="U25" s="5"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -3723,7 +3723,7 @@
       <c r="O26" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="P26" s="11"/>
+      <c r="P26" s="12"/>
       <c r="Q26" s="25"/>
       <c r="R26" s="25"/>
       <c r="S26" s="5"/>
@@ -3764,14 +3764,18 @@
       <c r="N27" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12" t="s">
-        <v>513</v>
+      <c r="O27" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="P27" s="11" t="s">
+        <v>260</v>
       </c>
       <c r="Q27" s="24"/>
       <c r="R27" s="24"/>
       <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
+      <c r="T27" s="5">
+        <v>4</v>
+      </c>
       <c r="U27" s="5"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
@@ -3988,7 +3992,7 @@
         <v>29</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="O32" s="11" t="s">
         <v>246</v>
@@ -4004,7 +4008,7 @@
         <v>4</v>
       </c>
       <c r="W32" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -4062,7 +4066,7 @@
         <v>425</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>543</v>
+        <v>568</v>
       </c>
       <c r="G34" s="4">
         <f t="shared" si="0"/>
@@ -4232,7 +4236,7 @@
         <v>544</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="G38" s="4">
         <f t="shared" si="0"/>
@@ -4274,7 +4278,7 @@
         <v>545</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G39" s="4">
         <f t="shared" si="0"/>
@@ -4316,7 +4320,7 @@
         <v>425</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G40" s="4">
         <f t="shared" si="0"/>
@@ -4395,7 +4399,7 @@
       <c r="T41" s="5"/>
       <c r="U41" s="5"/>
       <c r="W41" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
@@ -4606,14 +4610,18 @@
         <v>43</v>
       </c>
       <c r="N46" s="8"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="12" t="s">
-        <v>514</v>
+      <c r="O46" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="P46" s="11" t="s">
+        <v>261</v>
       </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="25"/>
       <c r="S46" s="5"/>
-      <c r="T46" s="5"/>
+      <c r="T46" s="5">
+        <v>5</v>
+      </c>
       <c r="U46" s="5"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
@@ -4754,7 +4762,9 @@
       <c r="C50" s="17" t="s">
         <v>427</v>
       </c>
-      <c r="D50" s="4"/>
+      <c r="D50" s="4" t="s">
+        <v>548</v>
+      </c>
       <c r="G50" s="4">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -4907,7 +4917,7 @@
         <v>50</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="O53" s="11" t="s">
         <v>246</v>
@@ -4921,7 +4931,7 @@
         <v>7</v>
       </c>
       <c r="W53" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
@@ -5164,7 +5174,7 @@
       <c r="N59" s="4"/>
       <c r="O59" s="11"/>
       <c r="P59" s="12" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="Q59" s="25"/>
       <c r="R59" s="25"/>
@@ -5172,7 +5182,7 @@
       <c r="T59" s="5"/>
       <c r="U59" s="5"/>
       <c r="W59" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update & new photos
</commit_message>
<xml_diff>
--- a/pin_map.xlsx
+++ b/pin_map.xlsx
@@ -11,11 +11,12 @@
     <sheet name="From-To" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="667">
   <si>
     <t>function</t>
   </si>
@@ -1929,6 +1930,93 @@
   </si>
   <si>
     <t>IN_RES3 (opt)</t>
+  </si>
+  <si>
+    <t>Lada-conn</t>
+  </si>
+  <si>
+    <t>* -&gt;db9_2</t>
+  </si>
+  <si>
+    <t>*-&gt;pwr_4</t>
+  </si>
+  <si>
+    <t>*-&gt;db9_1</t>
+  </si>
+  <si>
+    <t>* -&gt;db9_5</t>
+  </si>
+  <si>
+    <t>* -&gt;db9_6</t>
+  </si>
+  <si>
+    <t>* -&gt;db9_4</t>
+  </si>
+  <si>
+    <t>* -&gt;db9_3</t>
+  </si>
+  <si>
+    <t>*-&gt;pwr_1</t>
+  </si>
+  <si>
+    <t>*-&gt;pwr_2</t>
+  </si>
+  <si>
+    <t>*-&gt;pwr_7</t>
+  </si>
+  <si>
+    <t>*-&gt;pwr_6</t>
+  </si>
+  <si>
+    <t>*-&gt;pwr_8</t>
+  </si>
+  <si>
+    <t>*-&gt;lamb3</t>
+  </si>
+  <si>
+    <t>*-&gt;map3</t>
+  </si>
+  <si>
+    <t>*-&gt;map2</t>
+  </si>
+  <si>
+    <t>*-&gt;lamb1</t>
+  </si>
+  <si>
+    <t>*-&gt;map1</t>
+  </si>
+  <si>
+    <t>*-&gt;lamb4</t>
+  </si>
+  <si>
+    <t>*-&gt;stp4</t>
+  </si>
+  <si>
+    <t>*-&gt;stp3</t>
+  </si>
+  <si>
+    <t>*-&gt;stp2</t>
+  </si>
+  <si>
+    <t>*-&gt;stp1</t>
+  </si>
+  <si>
+    <t>*-&gt;ion1</t>
+  </si>
+  <si>
+    <t>*-&gt;ion2</t>
+  </si>
+  <si>
+    <t>*-&gt;ion3</t>
+  </si>
+  <si>
+    <t>*-&gt;ion4</t>
+  </si>
+  <si>
+    <t>*-&gt;lamb2</t>
+  </si>
+  <si>
+    <t>*screen</t>
   </si>
 </sst>
 </file>
@@ -2030,7 +2118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2064,6 +2152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2205,7 +2299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2312,6 +2406,11 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2619,8 +2718,8 @@
   </sheetPr>
   <dimension ref="A2:Y89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="K41" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="W56" sqref="W56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2645,6 +2744,7 @@
     <col min="19" max="20" width="4.28515625" customWidth="1"/>
     <col min="21" max="21" width="6.28515625" customWidth="1"/>
     <col min="22" max="22" width="5.85546875" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" style="67"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -2732,6 +2832,9 @@
       <c r="V3" s="59">
         <v>3410</v>
       </c>
+      <c r="W3" s="68" t="s">
+        <v>638</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
@@ -2772,6 +2875,9 @@
       </c>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
+      <c r="W4" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
@@ -2815,6 +2921,9 @@
       </c>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
+      <c r="W5" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
@@ -2856,6 +2965,9 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
+      <c r="W6" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
@@ -2896,6 +3008,9 @@
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
+      <c r="W7" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
@@ -2940,6 +3055,9 @@
       </c>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
+      <c r="W8" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
@@ -2986,6 +3104,9 @@
         <v>9</v>
       </c>
       <c r="V9" s="4"/>
+      <c r="W9" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -3036,6 +3157,9 @@
         <v>10</v>
       </c>
       <c r="V10" s="4"/>
+      <c r="W10" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -3086,6 +3210,9 @@
         <v>2</v>
       </c>
       <c r="V11" s="4"/>
+      <c r="W11" s="67" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -3274,6 +3401,9 @@
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
+      <c r="W15" s="67" t="s">
+        <v>648</v>
+      </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -3322,6 +3452,9 @@
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
+      <c r="W16" s="67" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -3370,6 +3503,9 @@
         <v>16</v>
       </c>
       <c r="V17" s="4"/>
+      <c r="W17" s="67" t="s">
+        <v>640</v>
+      </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
@@ -3418,6 +3554,9 @@
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
+      <c r="W18" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
@@ -3468,6 +3607,9 @@
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
+      <c r="W19" s="69" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -3514,6 +3656,9 @@
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
+      <c r="W20" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -3564,6 +3709,9 @@
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
+      <c r="W21" s="67" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -3640,6 +3788,9 @@
       </c>
       <c r="J23" s="10" t="s">
         <v>435</v>
+      </c>
+      <c r="K23">
+        <v>3</v>
       </c>
       <c r="L23" t="s">
         <v>631</v>
@@ -3687,6 +3838,9 @@
       <c r="J24" s="10" t="s">
         <v>436</v>
       </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
       <c r="M24" s="3">
         <v>21</v>
       </c>
@@ -3867,6 +4021,9 @@
       <c r="J28" s="10" t="s">
         <v>292</v>
       </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
       <c r="M28" s="3">
         <v>25</v>
       </c>
@@ -3914,6 +4071,9 @@
       <c r="J29" s="10" t="s">
         <v>291</v>
       </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
       <c r="L29" t="s">
         <v>631</v>
       </c>
@@ -3990,6 +4150,9 @@
         <v>12</v>
       </c>
       <c r="V30" s="4"/>
+      <c r="W30" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -4187,6 +4350,9 @@
         <v>5</v>
       </c>
       <c r="V34" s="4"/>
+      <c r="W34" s="67" t="s">
+        <v>641</v>
+      </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
@@ -4233,6 +4399,9 @@
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
       <c r="V35" s="4"/>
+      <c r="W35" s="67" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
@@ -4279,6 +4448,9 @@
       <c r="T36" s="4"/>
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
+      <c r="W36" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -4325,6 +4497,9 @@
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
+      <c r="W37" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
@@ -4371,6 +4546,9 @@
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
+      <c r="W38" s="67" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
@@ -4417,6 +4595,9 @@
       <c r="T39" s="4"/>
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
+      <c r="W39" s="67" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
@@ -4443,6 +4624,9 @@
       </c>
       <c r="J40" s="10" t="s">
         <v>296</v>
+      </c>
+      <c r="K40">
+        <v>7</v>
       </c>
       <c r="L40" t="s">
         <v>631</v>
@@ -4467,6 +4651,9 @@
       <c r="T40" s="4"/>
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
+      <c r="W40" s="67" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -4565,6 +4752,9 @@
       <c r="T42" s="4"/>
       <c r="U42" s="4"/>
       <c r="V42" s="4"/>
+      <c r="W42" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -4612,6 +4802,9 @@
       <c r="T43" s="4"/>
       <c r="U43" s="4"/>
       <c r="V43" s="4"/>
+      <c r="W43" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
@@ -4781,6 +4974,9 @@
       </c>
       <c r="J47" s="10" t="s">
         <v>297</v>
+      </c>
+      <c r="K47">
+        <v>4</v>
       </c>
       <c r="L47" t="s">
         <v>631</v>
@@ -4801,6 +4997,9 @@
       <c r="T47" s="4"/>
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
+      <c r="W47" s="67" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
@@ -4945,6 +5144,9 @@
         <v>11</v>
       </c>
       <c r="V50" s="4"/>
+      <c r="W50" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
@@ -4993,6 +5195,9 @@
         <v>15</v>
       </c>
       <c r="V51" s="4"/>
+      <c r="W51" s="67" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
@@ -5092,6 +5297,9 @@
         <v>3</v>
       </c>
       <c r="V53" s="4"/>
+      <c r="W53" s="67" t="s">
+        <v>649</v>
+      </c>
       <c r="X53" t="s">
         <v>518</v>
       </c>
@@ -5141,6 +5349,9 @@
       <c r="T54" s="4"/>
       <c r="U54" s="4"/>
       <c r="V54" s="4"/>
+      <c r="W54" s="67" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
@@ -5213,6 +5424,9 @@
       </c>
       <c r="J56" s="10" t="s">
         <v>295</v>
+      </c>
+      <c r="K56">
+        <v>6</v>
       </c>
       <c r="L56" t="s">
         <v>631</v>
@@ -5233,6 +5447,9 @@
       <c r="T56" s="4"/>
       <c r="U56" s="4"/>
       <c r="V56" s="4"/>
+      <c r="W56" s="67" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
@@ -5276,6 +5493,9 @@
       <c r="T57" s="4"/>
       <c r="U57" s="4"/>
       <c r="V57" s="4"/>
+      <c r="W57" s="67" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
@@ -5412,6 +5632,9 @@
       <c r="T60" s="4"/>
       <c r="U60" s="4"/>
       <c r="V60" s="4"/>
+      <c r="W60" s="67" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="28" t="s">
@@ -5505,6 +5728,9 @@
       <c r="T62" s="4"/>
       <c r="U62" s="4"/>
       <c r="V62" s="4"/>
+      <c r="W62" s="67" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="28" t="s">
@@ -5588,6 +5814,9 @@
       <c r="T64" s="4"/>
       <c r="U64" s="4"/>
       <c r="V64" s="4"/>
+      <c r="W64" s="67" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="28" t="s">
@@ -5716,6 +5945,9 @@
       <c r="T67" s="4"/>
       <c r="U67" s="4"/>
       <c r="V67" s="4"/>
+      <c r="W67" s="67" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" s="28" t="s">
@@ -5746,6 +5978,9 @@
       <c r="T68" s="4"/>
       <c r="U68" s="4"/>
       <c r="V68" s="4"/>
+      <c r="W68" s="67" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="28" t="s">
@@ -5779,6 +6014,9 @@
       <c r="T69" s="4"/>
       <c r="U69" s="4"/>
       <c r="V69" s="4"/>
+      <c r="W69" s="67" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="28" t="s">
@@ -5807,6 +6045,9 @@
       <c r="T70" s="4"/>
       <c r="U70" s="4"/>
       <c r="V70" s="4"/>
+      <c r="W70" s="67" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="28" t="s">
@@ -5845,6 +6086,9 @@
         <v>7</v>
       </c>
       <c r="V71" s="4"/>
+      <c r="W71" s="67" t="s">
+        <v>631</v>
+      </c>
       <c r="Y71" s="1" t="s">
         <v>237</v>
       </c>
@@ -5924,6 +6168,9 @@
         <v>6</v>
       </c>
       <c r="V73" s="4"/>
+      <c r="W73" s="67" t="s">
+        <v>650</v>
+      </c>
       <c r="Y73" t="s">
         <v>308</v>
       </c>
@@ -5965,6 +6212,9 @@
       <c r="T74" s="4"/>
       <c r="U74" s="4"/>
       <c r="V74" s="4"/>
+      <c r="W74" s="67" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="28" t="s">
@@ -6077,6 +6327,9 @@
       <c r="T77" s="4"/>
       <c r="U77" s="4"/>
       <c r="V77" s="4"/>
+      <c r="W77" s="67" t="s">
+        <v>661</v>
+      </c>
       <c r="Y77" t="s">
         <v>341</v>
       </c>
@@ -6116,6 +6369,9 @@
       <c r="T78" s="4"/>
       <c r="U78" s="4"/>
       <c r="V78" s="4"/>
+      <c r="W78" s="67" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="28" t="s">
@@ -6153,6 +6409,9 @@
       <c r="T79" s="4"/>
       <c r="U79" s="4"/>
       <c r="V79" s="4"/>
+      <c r="W79" s="67" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" s="28" t="s">
@@ -6192,8 +6451,11 @@
       <c r="T80" s="4"/>
       <c r="U80" s="4"/>
       <c r="V80" s="4"/>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W80" s="67" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" s="28" t="s">
         <v>94</v>
       </c>
@@ -6231,7 +6493,7 @@
       <c r="U81" s="4"/>
       <c r="V81" s="4"/>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" s="28" t="s">
         <v>95</v>
       </c>
@@ -6267,7 +6529,7 @@
       <c r="U82" s="4"/>
       <c r="V82" s="4"/>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" s="28" t="s">
         <v>75</v>
       </c>
@@ -6297,8 +6559,11 @@
       <c r="T83" s="4"/>
       <c r="U83" s="4"/>
       <c r="V83" s="4"/>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W83" s="67" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" s="28" t="s">
         <v>76</v>
       </c>
@@ -6330,7 +6595,7 @@
       <c r="U84" s="4"/>
       <c r="V84" s="4"/>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" s="28" t="s">
         <v>77</v>
       </c>
@@ -6348,7 +6613,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" s="28" t="s">
         <v>78</v>
       </c>
@@ -6368,7 +6633,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" s="28" t="s">
         <v>79</v>
       </c>
@@ -6388,7 +6653,7 @@
       <c r="Q87" s="14"/>
       <c r="R87" s="14"/>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
         <v>80</v>
       </c>
@@ -6400,7 +6665,7 @@
       </c>
       <c r="D88" s="28"/>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
         <v>81</v>
       </c>

</xml_diff>